<commit_message>
refactor code, add z_move function as unify entry point
</commit_message>
<xml_diff>
--- a/rampup.xlsx
+++ b/rampup.xlsx
@@ -429,100 +429,100 @@
                   <c:v>460</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>560</c:v>
+                  <c:v>660</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0">
-                  <c:v>724.63768115942025</c:v>
+                  <c:v>1063.8297872340424</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0">
-                  <c:v>869.56521739130437</c:v>
+                  <c:v>1265.8227848101267</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0">
-                  <c:v>1010.10101010101</c:v>
+                  <c:v>1515.1515151515152</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0">
-                  <c:v>1149.4252873563219</c:v>
+                  <c:v>1754.3859649122808</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0">
-                  <c:v>1282.051282051282</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0">
-                  <c:v>1388.8888888888889</c:v>
+                  <c:v>2173.913043478261</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0">
-                  <c:v>1492.5373134328358</c:v>
+                  <c:v>2380.9523809523807</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0">
-                  <c:v>1612.9032258064517</c:v>
+                  <c:v>2564.102564102564</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0">
-                  <c:v>1694.9152542372881</c:v>
+                  <c:v>2777.7777777777778</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0">
-                  <c:v>1785.7142857142858</c:v>
+                  <c:v>2941.1764705882351</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0">
-                  <c:v>1886.7924528301887</c:v>
+                  <c:v>3030.3030303030305</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0">
-                  <c:v>1960.7843137254902</c:v>
+                  <c:v>3225.8064516129034</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0">
-                  <c:v>2040.8163265306123</c:v>
+                  <c:v>3333.3333333333335</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0">
-                  <c:v>2127.6595744680849</c:v>
+                  <c:v>3448.2758620689656</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0">
-                  <c:v>2173.913043478261</c:v>
+                  <c:v>3571.4285714285716</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0">
-                  <c:v>2272.7272727272725</c:v>
+                  <c:v>3703.7037037037039</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0">
-                  <c:v>2325.5813953488373</c:v>
+                  <c:v>3846.1538461538462</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0">
-                  <c:v>2380.9523809523807</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>2439.0243902439024</c:v>
+                  <c:v>4166.666666666667</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0">
-                  <c:v>2500</c:v>
+                  <c:v>4166.666666666667</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0">
-                  <c:v>2564.102564102564</c:v>
+                  <c:v>4347.826086956522</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0">
-                  <c:v>2631.5789473684213</c:v>
+                  <c:v>4347.826086956522</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0">
-                  <c:v>2702.7027027027025</c:v>
+                  <c:v>4545.454545454545</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0">
-                  <c:v>2777.7777777777778</c:v>
+                  <c:v>4545.454545454545</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0">
-                  <c:v>2857.1428571428573</c:v>
+                  <c:v>4761.9047619047615</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0">
-                  <c:v>2857.1428571428573</c:v>
+                  <c:v>4761.9047619047615</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0">
-                  <c:v>2941.1764705882351</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0">
-                  <c:v>3030.3030303030305</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0">
-                  <c:v>3030.3030303030305</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0">
-                  <c:v>3125</c:v>
+                  <c:v>5263.1578947368425</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0">
-                  <c:v>3125</c:v>
+                  <c:v>5263.1578947368425</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -537,11 +537,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="471281208"/>
-        <c:axId val="471285128"/>
+        <c:axId val="289416224"/>
+        <c:axId val="289417008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="471281208"/>
+        <c:axId val="289416224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -597,12 +597,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471285128"/>
+        <c:crossAx val="289417008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="471285128"/>
+        <c:axId val="289417008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,7 +659,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471281208"/>
+        <c:crossAx val="289416224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -897,73 +897,73 @@
                   <c:v>217.39130434782609</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>178.57142857142858</c:v>
+                  <c:v>151.5151515151515</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>138.34289277321491</c:v>
+                  <c:v>94.38583563660174</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>95.979518909646728</c:v>
+                  <c:v>55.706562235410821</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>81.832801155820505</c:v>
+                  <c:v>47.754552447166198</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>73.064766959298083</c:v>
+                  <c:v>42.744962608104721</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>66.823913386462806</c:v>
+                  <c:v>39.15233125065545</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>62.049547491722727</c:v>
+                  <c:v>36.391558174916732</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>58.227150077040882</c:v>
+                  <c:v>34.174588334086621</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>55.068535865789684</c:v>
+                  <c:v>32.338609344273529</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>52.396572052410903</c:v>
+                  <c:v>30.782923672557846</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>50.094978630281744</c:v>
+                  <c:v>29.441124783008718</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>48.083559530682685</c:v>
+                  <c:v>28.267252020871918</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>46.304830418752893</c:v>
+                  <c:v>27.228268631221315</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>44.716287778717884</c:v>
+                  <c:v>26.299691654173255</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43.285691107945439</c:v>
+                  <c:v>25.462914524430218</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41.988054615185526</c:v>
+                  <c:v>24.703494283588896</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>40.803657767168296</c:v>
+                  <c:v>24.01001579177635</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>39.716688483419695</c:v>
+                  <c:v>23.373315324226542</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>38.714293062137308</c:v>
+                  <c:v>22.785935823305138</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>37.785895518939313</c:v>
+                  <c:v>22.241735943854433</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>36.922700072276527</c:v>
+                  <c:v>21.735603854384539</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>36.117321000422116</c:v>
+                  <c:v>21.263244019389543</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>35.363502885223333</c:v>
+                  <c:v>20.821015851814536</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1082,73 +1082,73 @@
                   <c:v>217.39130434782609</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>178.57142857142858</c:v>
+                  <c:v>151.5151515151515</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>138.34289277321491</c:v>
+                  <c:v>94.38583563660174</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>115.43829350726656</c:v>
+                  <c:v>79.48268575151036</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>98.696923820866502</c:v>
+                  <c:v>66.453241266215215</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>86.910530662384005</c:v>
+                  <c:v>57.067369115081931</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>78.311069786100461</c:v>
+                  <c:v>50.439332873534084</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>71.757992070382159</c:v>
+                  <c:v>45.572651207436998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>66.576646158925797</c:v>
+                  <c:v>41.842748011997344</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>62.357357982023991</c:v>
+                  <c:v>38.87994342047952</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>58.839843370313893</c:v>
+                  <c:v>36.458382429681933</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>55.851292053532248</c:v>
+                  <c:v>34.43363056561229</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>53.272449310734828</c:v>
+                  <c:v>32.709230244431446</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>51.018250519404361</c:v>
+                  <c:v>31.218280686132108</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>49.02628208857648</c:v>
+                  <c:v>29.912855907125362</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>47.249629214486426</c:v>
+                  <c:v>28.757662272295686</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>45.652283930310062</c:v>
+                  <c:v>27.726086469431653</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44.206103884835443</c:v>
+                  <c:v>26.797646318317632</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>42.888742192569659</c:v>
+                  <c:v>25.956295492355036</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41.682203723103179</c:v>
+                  <c:v>25.189265345892075</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>40.571816367376094</c:v>
+                  <c:v>24.486254605405446</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>39.545483794758347</c:v>
+                  <c:v>23.838850315878187</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>38.593133257141929</c:v>
+                  <c:v>23.240106152318887</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>37.706301155342246</c:v>
+                  <c:v>22.68423008190959</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1267,73 +1267,73 @@
                   <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>179</c:v>
+                  <c:v>152</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>138</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>115</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>99</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>87</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>78</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>67</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>62</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>59</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>56</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>53</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>51</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>49</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>47</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>46</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>42</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>40</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>39</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>38</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1348,11 +1348,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="471285912"/>
-        <c:axId val="404182160"/>
+        <c:axId val="291385864"/>
+        <c:axId val="291385080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="471285912"/>
+        <c:axId val="291385864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1409,12 +1409,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404182160"/>
+        <c:crossAx val="291385080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="404182160"/>
+        <c:axId val="291385080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1471,7 +1471,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471285912"/>
+        <c:crossAx val="291385864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1652,7 +1652,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1714,11 +1713,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="404182552"/>
-        <c:axId val="404179808"/>
+        <c:axId val="291384296"/>
+        <c:axId val="291379200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="404182552"/>
+        <c:axId val="291384296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1774,12 +1773,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404179808"/>
+        <c:crossAx val="291379200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="404179808"/>
+        <c:axId val="291379200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1836,7 +1835,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404182552"/>
+        <c:crossAx val="291384296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2059,11 +2058,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="404181768"/>
-        <c:axId val="404182944"/>
+        <c:axId val="291385472"/>
+        <c:axId val="291379984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="404181768"/>
+        <c:axId val="291385472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2119,12 +2118,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404182944"/>
+        <c:crossAx val="291379984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="404182944"/>
+        <c:axId val="291379984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2181,7 +2180,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404181768"/>
+        <c:crossAx val="291385472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4844,14 +4843,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R345"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" customWidth="1"/>
     <col min="3" max="4" width="12.1796875" customWidth="1"/>
     <col min="9" max="9" width="1.7265625" customWidth="1"/>
     <col min="10" max="10" width="6.7265625" customWidth="1"/>
@@ -4888,7 +4887,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>2000</v>
+        <v>6000</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -4954,58 +4953,58 @@
       <c r="A4" s="7"/>
       <c r="D4" s="3">
         <f t="shared" si="1"/>
-        <v>38.81987577639751</v>
+        <v>65.876152832674592</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4" s="16">
         <f>$B$12/J4</f>
-        <v>178.57142857142858</v>
+        <v>151.5151515151515</v>
       </c>
       <c r="G4" s="3">
         <f>$B$12/J4</f>
-        <v>178.57142857142858</v>
+        <v>151.5151515151515</v>
       </c>
       <c r="H4" s="14">
         <f>ROUND(G4,0)</f>
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="J4" s="15">
-        <v>560</v>
+        <v>660</v>
       </c>
       <c r="K4" s="4">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D5" s="3">
         <f t="shared" si="1"/>
-        <v>40.22853579821367</v>
+        <v>57.129315878549761</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5" s="16">
         <f>B17</f>
-        <v>138.34289277321491</v>
+        <v>94.38583563660174</v>
       </c>
       <c r="G5" s="3">
         <f>B17</f>
-        <v>138.34289277321491</v>
+        <v>94.38583563660174</v>
       </c>
       <c r="H5" s="8">
         <f>ROUND(G5,0)</f>
-        <v>138</v>
+        <v>94</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" ref="J5:J35" si="3">$B$12/H5</f>
-        <v>724.63768115942025</v>
+        <v>1063.8297872340424</v>
       </c>
       <c r="K5" s="4">
         <f t="shared" si="2"/>
-        <v>164.63768115942025</v>
+        <v>403.82978723404244</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -5017,34 +5016,34 @@
       </c>
       <c r="D6" s="3">
         <f>G5-G6</f>
-        <v>22.904599265948349</v>
+        <v>14.903149885091381</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6" s="16">
         <f t="shared" ref="F6:F35" si="4">F5*(1+-1*$B$22*F5*F5)</f>
-        <v>95.979518909646728</v>
+        <v>55.706562235410821</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G35" si="5">G5*(1+I6+1.5*I6*I6)</f>
-        <v>115.43829350726656</v>
+        <v>79.48268575151036</v>
       </c>
       <c r="H6" s="8">
         <f t="shared" ref="H6:H35" si="6">ROUND(G6,0)</f>
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" ref="I6:I35" si="7">-1*$B$22*G5*G5</f>
-        <v>-0.30622009569377978</v>
+        <v>-0.40979955456570155</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="3"/>
-        <v>869.56521739130437</v>
+        <v>1265.8227848101267</v>
       </c>
       <c r="K6" s="4">
         <f>J6-J5</f>
-        <v>144.92753623188412</v>
+        <v>201.99299757608424</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -5057,34 +5056,34 @@
       </c>
       <c r="D7" s="3">
         <f t="shared" ref="D7:D37" si="8">G6-G7</f>
-        <v>16.741369686400063</v>
+        <v>13.029444485295144</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7" s="16">
         <f t="shared" si="4"/>
-        <v>81.832801155820505</v>
+        <v>47.754552447166198</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" si="5"/>
-        <v>98.696923820866502</v>
+        <v>66.453241266215215</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" si="6"/>
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="7"/>
-        <v>-0.21321599372591715</v>
+        <v>-0.29060487737657403</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="3"/>
-        <v>1010.10101010101</v>
+        <v>1515.1515151515152</v>
       </c>
       <c r="K7" s="4">
         <f t="shared" ref="K7:K35" si="9">J7-J6</f>
-        <v>140.53579270970567</v>
+        <v>249.32873034138856</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -5093,34 +5092,34 @@
       </c>
       <c r="D8" s="3">
         <f t="shared" si="8"/>
-        <v>11.786393158482497</v>
+        <v>9.3858721511332845</v>
       </c>
       <c r="E8">
         <v>7</v>
       </c>
       <c r="F8" s="16">
         <f t="shared" si="4"/>
-        <v>73.064766959298083</v>
+        <v>42.744962608104721</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" si="5"/>
-        <v>86.910530662384005</v>
+        <v>57.067369115081931</v>
       </c>
       <c r="H8" s="8">
         <f t="shared" si="6"/>
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="7"/>
-        <v>-0.15585732434723082</v>
+        <v>-0.20313753064014722</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="3"/>
-        <v>1149.4252873563219</v>
+        <v>1754.3859649122808</v>
       </c>
       <c r="K8" s="4">
         <f t="shared" si="9"/>
-        <v>139.32427725531181</v>
+        <v>239.23444976076553</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -5136,34 +5135,34 @@
       </c>
       <c r="D9" s="3">
         <f t="shared" si="8"/>
-        <v>8.5994608762835441</v>
+        <v>6.6280362415478464</v>
       </c>
       <c r="E9">
         <v>8</v>
       </c>
       <c r="F9" s="16">
         <f t="shared" si="4"/>
-        <v>66.823913386462806</v>
+        <v>39.15233125065545</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" si="5"/>
-        <v>78.311069786100461</v>
+        <v>50.439332873534084</v>
       </c>
       <c r="H9" s="8">
         <f t="shared" si="6"/>
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="7"/>
-        <v>-0.12085504544027503</v>
+        <v>-0.14980749241498231</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="3"/>
-        <v>1282.051282051282</v>
+        <v>2000</v>
       </c>
       <c r="K9" s="4">
         <f t="shared" si="9"/>
-        <v>132.62599469496013</v>
+        <v>245.61403508771923</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -5172,41 +5171,41 @@
       </c>
       <c r="B10">
         <f>B2</f>
-        <v>2000</v>
+        <v>6000</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="8"/>
-        <v>6.5530777157183024</v>
+        <v>4.8666816660970866</v>
       </c>
       <c r="E10">
         <v>9</v>
       </c>
       <c r="F10" s="16">
         <f t="shared" si="4"/>
-        <v>62.049547491722727</v>
+        <v>36.391558174916732</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" si="5"/>
-        <v>71.757992070382159</v>
+        <v>45.572651207436998</v>
       </c>
       <c r="H10" s="8">
         <f t="shared" si="6"/>
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" si="7"/>
-        <v>-9.812197841669594E-2</v>
+        <v>-0.1170298098334501</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="3"/>
-        <v>1388.8888888888889</v>
+        <v>2173.913043478261</v>
       </c>
       <c r="K10" s="4">
         <f t="shared" si="9"/>
-        <v>106.83760683760693</v>
+        <v>173.91304347826099</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -5214,41 +5213,41 @@
         <v>7</v>
       </c>
       <c r="B11" s="7">
-        <v>160000</v>
+        <v>460000</v>
       </c>
       <c r="C11" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="8"/>
-        <v>5.1813459114563614</v>
+        <v>3.729903195439654</v>
       </c>
       <c r="E11">
         <v>10</v>
       </c>
       <c r="F11" s="16">
         <f t="shared" si="4"/>
-        <v>58.227150077040882</v>
+        <v>34.174588334086621</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" si="5"/>
-        <v>66.576646158925797</v>
+        <v>41.842748011997344</v>
       </c>
       <c r="H11" s="8">
         <f t="shared" si="6"/>
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" si="7"/>
-        <v>-8.2387350815568458E-2</v>
+        <v>-9.5535860751436608E-2</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="3"/>
-        <v>1492.5373134328358</v>
+        <v>2380.9523809523807</v>
       </c>
       <c r="K11" s="4">
         <f t="shared" si="9"/>
-        <v>103.64842454394693</v>
+        <v>207.03933747411975</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -5263,34 +5262,34 @@
       </c>
       <c r="D12" s="3">
         <f t="shared" si="8"/>
-        <v>4.2192881769018058</v>
+        <v>2.9628045915178234</v>
       </c>
       <c r="E12">
         <v>11</v>
       </c>
       <c r="F12" s="16">
         <f t="shared" si="4"/>
-        <v>55.068535865789684</v>
+        <v>32.338609344273529</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="5"/>
-        <v>62.357357982023991</v>
+        <v>38.87994342047952</v>
       </c>
       <c r="H12" s="8">
         <f t="shared" si="6"/>
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" si="7"/>
-        <v>-7.0919197020332947E-2</v>
+        <v>-8.0537515814993355E-2</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="3"/>
-        <v>1612.9032258064517</v>
+        <v>2564.102564102564</v>
       </c>
       <c r="K12" s="4">
         <f t="shared" si="9"/>
-        <v>120.36591237361586</v>
+        <v>183.15018315018324</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -5299,34 +5298,34 @@
       </c>
       <c r="D13" s="3">
         <f t="shared" si="8"/>
-        <v>3.5175146117100979</v>
+        <v>2.4215609907975875</v>
       </c>
       <c r="E13">
         <v>12</v>
       </c>
       <c r="F13" s="16">
         <f t="shared" si="4"/>
-        <v>52.396572052410903</v>
+        <v>30.782923672557846</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="5"/>
-        <v>58.839843370313893</v>
+        <v>36.458382429681933</v>
       </c>
       <c r="H13" s="8">
         <f t="shared" si="6"/>
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="7"/>
-        <v>-6.2215041511972657E-2</v>
+        <v>-6.9535900017465679E-2</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="3"/>
-        <v>1694.9152542372881</v>
+        <v>2777.7777777777778</v>
       </c>
       <c r="K13" s="4">
         <f t="shared" si="9"/>
-        <v>82.012028430836381</v>
+        <v>213.67521367521385</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -5335,34 +5334,34 @@
       </c>
       <c r="D14" s="3">
         <f t="shared" si="8"/>
-        <v>2.9885513167816455</v>
+        <v>2.0247518640696427</v>
       </c>
       <c r="E14">
         <v>13</v>
       </c>
       <c r="F14" s="16">
         <f t="shared" si="4"/>
-        <v>50.094978630281744</v>
+        <v>29.441124783008718</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="5"/>
-        <v>55.851292053532248</v>
+        <v>34.43363056561229</v>
       </c>
       <c r="H14" s="8">
         <f t="shared" si="6"/>
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="7"/>
-        <v>-5.5394034685489146E-2</v>
+        <v>-6.1143827871891251E-2</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="3"/>
-        <v>1785.7142857142858</v>
+        <v>2941.1764705882351</v>
       </c>
       <c r="K14" s="4">
         <f t="shared" si="9"/>
-        <v>90.799031476997698</v>
+        <v>163.39869281045731</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -5371,38 +5370,38 @@
       </c>
       <c r="B15" s="4">
         <f>(B10*B10-B9*B9)/(2*B11)</f>
-        <v>11.8671875</v>
+        <v>38.910326086956523</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" si="8"/>
-        <v>2.5788427427974199</v>
+        <v>1.7244003211808447</v>
       </c>
       <c r="E15">
         <v>14</v>
       </c>
       <c r="F15" s="16">
         <f t="shared" si="4"/>
-        <v>48.083559530682685</v>
+        <v>28.267252020871918</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="5"/>
-        <v>53.272449310734828</v>
+        <v>32.709230244431446</v>
       </c>
       <c r="H15" s="8">
         <f t="shared" si="6"/>
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="I15" s="2">
         <f t="shared" si="7"/>
-        <v>-4.9909869184783275E-2</v>
+        <v>-5.4541046040737173E-2</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="3"/>
-        <v>1886.7924528301887</v>
+        <v>3030.3030303030305</v>
       </c>
       <c r="K15" s="4">
         <f t="shared" si="9"/>
-        <v>101.07816711590294</v>
+        <v>89.126559714795349</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -5411,34 +5410,34 @@
       </c>
       <c r="D16" s="3">
         <f t="shared" si="8"/>
-        <v>2.2541987913304666</v>
+        <v>1.490949558299338</v>
       </c>
       <c r="E16">
         <v>15</v>
       </c>
       <c r="F16" s="16">
         <f t="shared" si="4"/>
-        <v>46.304830418752893</v>
+        <v>27.228268631221315</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="5"/>
-        <v>51.018250519404361</v>
+        <v>31.218280686132108</v>
       </c>
       <c r="H16" s="8">
         <f t="shared" si="6"/>
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="7"/>
-        <v>-4.5407261689036985E-2</v>
+        <v>-4.9215112186428524E-2</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" si="3"/>
-        <v>1960.7843137254902</v>
+        <v>3225.8064516129034</v>
       </c>
       <c r="K16" s="4">
         <f t="shared" si="9"/>
-        <v>73.991860895301443</v>
+        <v>195.50342130987292</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -5447,71 +5446,71 @@
       </c>
       <c r="B17" s="3">
         <f>B12/SQRT(B9*B9+2*B11)</f>
-        <v>138.34289277321491</v>
+        <v>94.38583563660174</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="8"/>
-        <v>1.9919684308278818</v>
+        <v>1.3054247790067457</v>
       </c>
       <c r="E17">
         <v>16</v>
       </c>
       <c r="F17" s="16">
         <f t="shared" si="4"/>
-        <v>44.716287778717884</v>
+        <v>26.299691654173255</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="5"/>
-        <v>49.02628208857648</v>
+        <v>29.912855907125362</v>
       </c>
       <c r="H17" s="8">
         <f t="shared" si="6"/>
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="I17" s="2">
         <f t="shared" si="7"/>
-        <v>-4.1645790176971252E-2</v>
+        <v>-4.4830728253913932E-2</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="3"/>
-        <v>2040.8163265306123</v>
+        <v>3333.3333333333335</v>
       </c>
       <c r="K17" s="4">
         <f t="shared" si="9"/>
-        <v>80.032012805122122</v>
+        <v>107.52688172043008</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D18" s="3">
         <f t="shared" si="8"/>
-        <v>1.776652874090054</v>
+        <v>1.1551936348296756</v>
       </c>
       <c r="E18">
         <v>17</v>
       </c>
       <c r="F18" s="16">
         <f t="shared" si="4"/>
-        <v>43.285691107945439</v>
+        <v>25.462914524430218</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="5"/>
-        <v>47.249629214486426</v>
+        <v>28.757662272295686</v>
       </c>
       <c r="H18" s="8">
         <f t="shared" si="6"/>
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" si="7"/>
-        <v>-3.84572213668588E-2</v>
+        <v>-4.1159831631940452E-2</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" si="3"/>
-        <v>2127.6595744680849</v>
+        <v>3448.2758620689656</v>
       </c>
       <c r="K18" s="4">
         <f t="shared" si="9"/>
-        <v>86.843247937472597</v>
+        <v>114.9425287356321</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -5520,34 +5519,34 @@
       </c>
       <c r="D19" s="3">
         <f t="shared" si="8"/>
-        <v>1.5973452841763631</v>
+        <v>1.0315758028640332</v>
       </c>
       <c r="E19">
         <v>18</v>
       </c>
       <c r="F19" s="16">
         <f t="shared" si="4"/>
-        <v>41.988054615185526</v>
+        <v>24.703494283588896</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" si="5"/>
-        <v>45.652283930310062</v>
+        <v>27.726086469431653</v>
       </c>
       <c r="H19" s="8">
         <f t="shared" si="6"/>
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" si="7"/>
-        <v>-3.5720439374503185E-2</v>
+        <v>-3.8042144410901257E-2</v>
       </c>
       <c r="J19" s="4">
         <f t="shared" si="3"/>
-        <v>2173.913043478261</v>
+        <v>3571.4285714285716</v>
       </c>
       <c r="K19" s="4">
         <f t="shared" si="9"/>
-        <v>46.253469010176104</v>
+        <v>123.15270935960598</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -5556,38 +5555,38 @@
       </c>
       <c r="B20" s="3">
         <f>B12/B10</f>
-        <v>50</v>
+        <v>16.666666666666668</v>
       </c>
       <c r="D20" s="3">
         <f t="shared" si="8"/>
-        <v>1.4461800454746196</v>
+        <v>0.92844015111402101</v>
       </c>
       <c r="E20">
         <v>19</v>
       </c>
       <c r="F20" s="16">
         <f t="shared" si="4"/>
-        <v>40.803657767168296</v>
+        <v>24.01001579177635</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" si="5"/>
-        <v>44.206103884835443</v>
+        <v>26.797646318317632</v>
       </c>
       <c r="H20" s="8">
         <f t="shared" si="6"/>
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" si="7"/>
-        <v>-3.3346096448858338E-2</v>
+        <v>-3.5361850061878447E-2</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" si="3"/>
-        <v>2272.7272727272725</v>
+        <v>3703.7037037037039</v>
       </c>
       <c r="K20" s="4">
         <f t="shared" si="9"/>
-        <v>98.814229249011532</v>
+        <v>132.27513227513236</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -5596,34 +5595,34 @@
       </c>
       <c r="D21" s="3">
         <f t="shared" si="8"/>
-        <v>1.3173616922657843</v>
+        <v>0.84135082596259636</v>
       </c>
       <c r="E21">
         <v>20</v>
       </c>
       <c r="F21" s="16">
         <f t="shared" si="4"/>
-        <v>39.716688483419695</v>
+        <v>23.373315324226542</v>
       </c>
       <c r="G21" s="3">
         <f t="shared" si="5"/>
-        <v>42.888742192569659</v>
+        <v>25.956295492355036</v>
       </c>
       <c r="H21" s="8">
         <f t="shared" si="6"/>
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="I21" s="2">
         <f t="shared" si="7"/>
-        <v>-3.126687393082981E-2</v>
+        <v>-3.3033237017275556E-2</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" si="3"/>
-        <v>2325.5813953488373</v>
+        <v>3846.1538461538462</v>
       </c>
       <c r="K21" s="4">
         <f t="shared" si="9"/>
-        <v>52.854122621564784</v>
+        <v>142.45014245014227</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -5632,38 +5631,38 @@
       </c>
       <c r="B22">
         <f>B11/(B12*B12)</f>
-        <v>1.5999999999999999E-5</v>
+        <v>4.6E-5</v>
       </c>
       <c r="D22" s="3">
         <f t="shared" si="8"/>
-        <v>1.20653846946648</v>
+        <v>0.76703014646296097</v>
       </c>
       <c r="E22">
         <v>21</v>
       </c>
       <c r="F22" s="16">
         <f t="shared" si="4"/>
-        <v>38.714293062137308</v>
+        <v>22.785935823305138</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="5"/>
-        <v>41.682203723103179</v>
+        <v>25.189265345892075</v>
       </c>
       <c r="H22" s="8">
         <f t="shared" si="6"/>
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" si="7"/>
-        <v>-2.9431107309771276E-2</v>
+        <v>-3.0991546681576713E-2</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" si="3"/>
-        <v>2380.9523809523807</v>
+        <v>4000</v>
       </c>
       <c r="K22" s="4">
         <f t="shared" si="9"/>
-        <v>55.370985603543431</v>
+        <v>153.84615384615381</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -5672,34 +5671,34 @@
       </c>
       <c r="D23" s="3">
         <f t="shared" si="8"/>
-        <v>1.1103873557270845</v>
+        <v>0.70301074048662926</v>
       </c>
       <c r="E23">
         <v>22</v>
       </c>
       <c r="F23" s="16">
         <f t="shared" si="4"/>
-        <v>37.785895518939313</v>
+        <v>22.241735943854433</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" si="5"/>
-        <v>40.571816367376094</v>
+        <v>24.486254605405446</v>
       </c>
       <c r="H23" s="8">
         <f t="shared" si="6"/>
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="I23" s="2">
         <f t="shared" si="7"/>
-        <v>-2.7798497715428423E-2</v>
+        <v>-2.9186958078624932E-2</v>
       </c>
       <c r="J23" s="4">
         <f t="shared" si="3"/>
-        <v>2439.0243902439024</v>
+        <v>4166.666666666667</v>
       </c>
       <c r="K23" s="4">
         <f t="shared" si="9"/>
-        <v>58.072009291521681</v>
+        <v>166.66666666666697</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -5708,34 +5707,34 @@
       </c>
       <c r="D24" s="3">
         <f t="shared" si="8"/>
-        <v>1.026332572617747</v>
+        <v>0.64740428952725892</v>
       </c>
       <c r="E24">
         <v>23</v>
       </c>
       <c r="F24" s="16">
         <f t="shared" si="4"/>
-        <v>36.922700072276527</v>
+        <v>21.735603854384539</v>
       </c>
       <c r="G24" s="3">
         <f t="shared" si="5"/>
-        <v>39.545483794758347</v>
+        <v>23.838850315878187</v>
       </c>
       <c r="H24" s="8">
         <f t="shared" si="6"/>
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="I24" s="2">
         <f t="shared" si="7"/>
-        <v>-2.6337156533569387E-2</v>
+        <v>-2.7580526571634009E-2</v>
       </c>
       <c r="J24" s="4">
         <f t="shared" si="3"/>
-        <v>2500</v>
+        <v>4166.666666666667</v>
       </c>
       <c r="K24" s="4">
         <f t="shared" si="9"/>
-        <v>60.975609756097583</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -5744,34 +5743,34 @@
       </c>
       <c r="D25" s="3">
         <f t="shared" si="8"/>
-        <v>0.95235053761641808</v>
+        <v>0.59874416355929938</v>
       </c>
       <c r="E25">
         <v>24</v>
       </c>
       <c r="F25" s="16">
         <f t="shared" si="4"/>
-        <v>36.117321000422116</v>
+        <v>21.263244019389543</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" si="5"/>
-        <v>38.593133257141929</v>
+        <v>23.240106152318887</v>
       </c>
       <c r="H25" s="8">
         <f t="shared" si="6"/>
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="I25" s="2">
         <f t="shared" si="7"/>
-        <v>-2.5021524616983919E-2</v>
+        <v>-2.6141376081610896E-2</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" si="3"/>
-        <v>2564.102564102564</v>
+        <v>4347.826086956522</v>
       </c>
       <c r="K25" s="4">
         <f t="shared" si="9"/>
-        <v>64.102564102563974</v>
+        <v>181.15942028985501</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -5780,34 +5779,34 @@
       </c>
       <c r="D26" s="3">
         <f t="shared" si="8"/>
-        <v>0.88683210179968341</v>
+        <v>0.55587607040929754</v>
       </c>
       <c r="E26">
         <v>25</v>
       </c>
       <c r="F26" s="16">
         <f t="shared" si="4"/>
-        <v>35.363502885223333</v>
+        <v>20.821015851814536</v>
       </c>
       <c r="G26" s="3">
         <f t="shared" si="5"/>
-        <v>37.706301155342246</v>
+        <v>22.68423008190959</v>
       </c>
       <c r="H26" s="8">
         <f t="shared" si="6"/>
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="I26" s="2">
         <f t="shared" si="7"/>
-        <v>-2.383087895365623E-2</v>
+        <v>-2.4844716562668307E-2</v>
       </c>
       <c r="J26" s="4">
         <f t="shared" si="3"/>
-        <v>2631.5789473684213</v>
+        <v>4347.826086956522</v>
       </c>
       <c r="K26" s="4">
         <f t="shared" si="9"/>
-        <v>67.476383265857294</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -5816,34 +5815,34 @@
       </c>
       <c r="D27" s="3">
         <f t="shared" si="8"/>
-        <v>0.82848354859238782</v>
+        <v>0.51788062213616826</v>
       </c>
       <c r="E27">
         <v>26</v>
       </c>
       <c r="F27" s="16">
         <f t="shared" si="4"/>
-        <v>34.655906161368826</v>
+        <v>20.405809894487593</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="5"/>
-        <v>36.877817606749858</v>
+        <v>22.166349459773421</v>
       </c>
       <c r="H27" s="8">
         <f t="shared" si="6"/>
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="I27" s="2">
         <f t="shared" si="7"/>
-        <v>-2.2748242349077821E-2</v>
+        <v>-2.3670417542814549E-2</v>
       </c>
       <c r="J27" s="4">
         <f t="shared" si="3"/>
-        <v>2702.7027027027025</v>
+        <v>4545.454545454545</v>
       </c>
       <c r="K27" s="4">
         <f t="shared" si="9"/>
-        <v>71.123755334281213</v>
+        <v>197.62845849802306</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -5852,34 +5851,34 @@
       </c>
       <c r="D28" s="3">
         <f t="shared" si="8"/>
-        <v>0.77625432063945254</v>
+        <v>0.48401755839681826</v>
       </c>
       <c r="E28">
         <v>27</v>
       </c>
       <c r="F28" s="16">
         <f t="shared" si="4"/>
-        <v>33.989940617977609</v>
+        <v>20.014951592746637</v>
       </c>
       <c r="G28" s="3">
         <f t="shared" si="5"/>
-        <v>36.101563286110405</v>
+        <v>21.682331901376603</v>
       </c>
       <c r="H28" s="8">
         <f t="shared" si="6"/>
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="I28" s="2">
         <f t="shared" si="7"/>
-        <v>-2.1759574902987355E-2</v>
+        <v>-2.2601964225148683E-2</v>
       </c>
       <c r="J28" s="4">
         <f t="shared" si="3"/>
-        <v>2777.7777777777778</v>
+        <v>4545.454545454545</v>
       </c>
       <c r="K28" s="4">
         <f t="shared" si="9"/>
-        <v>75.075075075075347</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -5888,34 +5887,34 @@
       </c>
       <c r="D29" s="3">
         <f t="shared" si="8"/>
-        <v>0.72928349765543032</v>
+        <v>0.45368494179322738</v>
       </c>
       <c r="E29">
         <v>28</v>
       </c>
       <c r="F29" s="16">
         <f t="shared" si="4"/>
-        <v>33.361634627839571</v>
+        <v>19.646125647674925</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="5"/>
-        <v>35.372279788454975</v>
+        <v>21.228646959583376</v>
       </c>
       <c r="H29" s="8">
         <f t="shared" si="6"/>
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="I29" s="2">
         <f t="shared" si="7"/>
-        <v>-2.0853165947216555E-2</v>
+        <v>-2.1625681767346864E-2</v>
       </c>
       <c r="J29" s="4">
         <f t="shared" si="3"/>
-        <v>2857.1428571428573</v>
+        <v>4761.9047619047615</v>
       </c>
       <c r="K29" s="4">
         <f t="shared" si="9"/>
-        <v>79.365079365079509</v>
+        <v>216.45021645021643</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -5924,30 +5923,30 @@
       </c>
       <c r="D30" s="3">
         <f t="shared" si="8"/>
-        <v>0.68685963769743807</v>
+        <v>0.42638888122998253</v>
       </c>
       <c r="E30">
         <v>29</v>
       </c>
       <c r="F30" s="16">
         <f t="shared" si="4"/>
-        <v>32.767531350969385</v>
+        <v>19.297315923718919</v>
       </c>
       <c r="G30" s="3">
         <f t="shared" si="5"/>
-        <v>34.685420150757537</v>
+        <v>20.802258078353393</v>
       </c>
       <c r="H30" s="8">
         <f t="shared" si="6"/>
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="I30" s="2">
         <f t="shared" si="7"/>
-        <v>-2.0019170838923843E-2</v>
+        <v>-2.073015077979291E-2</v>
       </c>
       <c r="J30" s="4">
         <f t="shared" si="3"/>
-        <v>2857.1428571428573</v>
+        <v>4761.9047619047615</v>
       </c>
       <c r="K30" s="4">
         <f t="shared" si="9"/>
@@ -5960,34 +5959,34 @@
       </c>
       <c r="D31" s="3">
         <f t="shared" si="8"/>
-        <v>0.64839028076910665</v>
+        <v>0.40172077438071341</v>
       </c>
       <c r="E31">
         <v>30</v>
       </c>
       <c r="F31" s="16">
         <f t="shared" si="4"/>
-        <v>32.204605551189744</v>
+        <v>18.96675725376917</v>
       </c>
       <c r="G31" s="3">
         <f t="shared" si="5"/>
-        <v>34.03702986998843</v>
+        <v>20.40053730397268</v>
       </c>
       <c r="H31" s="8">
         <f t="shared" si="6"/>
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" si="7"/>
-        <v>-1.9249253936553228E-2</v>
+        <v>-1.9905761293287274E-2</v>
       </c>
       <c r="J31" s="4">
         <f t="shared" si="3"/>
-        <v>2941.1764705882351</v>
+        <v>5000</v>
       </c>
       <c r="K31" s="4">
         <f t="shared" si="9"/>
-        <v>84.033613445377796</v>
+        <v>238.09523809523853</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -5996,34 +5995,34 @@
       </c>
       <c r="D32" s="3">
         <f t="shared" si="8"/>
-        <v>0.61337853211149707</v>
+        <v>0.3793399974568672</v>
       </c>
       <c r="E32">
         <v>31</v>
       </c>
       <c r="F32" s="16">
         <f t="shared" si="4"/>
-        <v>31.670196339858915</v>
+        <v>18.652896445070525</v>
       </c>
       <c r="G32" s="3">
         <f t="shared" si="5"/>
-        <v>33.423651337876933</v>
+        <v>20.021197306515813</v>
       </c>
       <c r="H32" s="8">
         <f t="shared" si="6"/>
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="I32" s="2">
         <f t="shared" si="7"/>
-        <v>-1.8536310437927753E-2</v>
+        <v>-1.914436842537592E-2</v>
       </c>
       <c r="J32" s="4">
         <f t="shared" si="3"/>
-        <v>3030.3030303030305</v>
+        <v>5000</v>
       </c>
       <c r="K32" s="4">
         <f t="shared" si="9"/>
-        <v>89.126559714795349</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
@@ -6032,30 +6031,30 @@
       </c>
       <c r="D33" s="3">
         <f t="shared" si="8"/>
-        <v>0.58140489680937435</v>
+        <v>0.35896059348251441</v>
       </c>
       <c r="E33">
         <v>32</v>
       </c>
       <c r="F33" s="16">
         <f t="shared" si="4"/>
-        <v>31.161952351910756</v>
+        <v>18.354360472797978</v>
       </c>
       <c r="G33" s="3">
         <f t="shared" si="5"/>
-        <v>32.842246441067559</v>
+        <v>19.662236713033298</v>
       </c>
       <c r="H33" s="8">
         <f t="shared" si="6"/>
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="I33" s="2">
         <f t="shared" si="7"/>
-        <v>-1.7874247500095398E-2</v>
+        <v>-1.8439023712976059E-2</v>
       </c>
       <c r="J33" s="4">
         <f t="shared" si="3"/>
-        <v>3030.3030303030305</v>
+        <v>5000</v>
       </c>
       <c r="K33" s="4">
         <f t="shared" si="9"/>
@@ -6065,34 +6064,34 @@
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="D34" s="3">
         <f t="shared" si="8"/>
-        <v>0.55211305394710308</v>
+        <v>0.3403409313903083</v>
       </c>
       <c r="E34">
         <v>33</v>
       </c>
       <c r="F34" s="16">
         <f t="shared" si="4"/>
-        <v>30.677786717753708</v>
+        <v>18.069930341232077</v>
       </c>
       <c r="G34" s="3">
         <f t="shared" si="5"/>
-        <v>32.290133387120456</v>
+        <v>19.32189578164299</v>
       </c>
       <c r="H34" s="8">
         <f t="shared" si="6"/>
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I34" s="2">
         <f t="shared" si="7"/>
-        <v>-1.7257810420733037E-2</v>
+        <v>-1.7783763417730306E-2</v>
       </c>
       <c r="J34" s="4">
         <f t="shared" si="3"/>
-        <v>3125</v>
+        <v>5263.1578947368425</v>
       </c>
       <c r="K34" s="4">
         <f t="shared" si="9"/>
-        <v>94.696969696969518</v>
+        <v>263.15789473684254</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6101,30 +6100,30 @@
       </c>
       <c r="D35" s="3">
         <f t="shared" si="8"/>
-        <v>0.5251986174812231</v>
+        <v>0.32327559728410193</v>
       </c>
       <c r="E35">
         <v>34</v>
       </c>
       <c r="F35" s="16">
         <f t="shared" si="4"/>
-        <v>30.215839821037214</v>
+        <v>17.798519452696446</v>
       </c>
       <c r="G35" s="3">
         <f t="shared" si="5"/>
-        <v>31.764934769639233</v>
+        <v>18.998620184358888</v>
       </c>
       <c r="H35" s="9">
         <f t="shared" si="6"/>
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I35" s="2">
         <f t="shared" si="7"/>
-        <v>-1.6682443426528495E-2</v>
+        <v>-1.7173440203446966E-2</v>
       </c>
       <c r="J35" s="4">
         <f t="shared" si="3"/>
-        <v>3125</v>
+        <v>5263.1578947368425</v>
       </c>
       <c r="K35" s="4">
         <f t="shared" si="9"/>
@@ -6137,7 +6136,7 @@
       </c>
       <c r="D36" s="3">
         <f t="shared" si="8"/>
-        <v>31.764934769639233</v>
+        <v>18.998620184358888</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
start to merge sync and async code into one
</commit_message>
<xml_diff>
--- a/rampup.xlsx
+++ b/rampup.xlsx
@@ -13,7 +13,11 @@
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>pps</t>
   </si>
@@ -145,17 +149,68 @@
   <si>
     <t>p(ARR) better</t>
   </si>
+  <si>
+    <t>ARR_8_24 format</t>
+  </si>
+  <si>
+    <t>rev/m</t>
+  </si>
+  <si>
+    <t>rev/sec</t>
+  </si>
+  <si>
+    <t>tread pitch to cut</t>
+  </si>
+  <si>
+    <t>ARR</t>
+  </si>
+  <si>
+    <t>steps/per mm setup</t>
+  </si>
+  <si>
+    <t>steps/sec</t>
+  </si>
+  <si>
+    <t>encoder*2</t>
+  </si>
+  <si>
+    <t>HZ spindle encoder</t>
+  </si>
+  <si>
+    <t>mm per spindle step</t>
+  </si>
+  <si>
+    <t>steps to accelerate to 4000</t>
+  </si>
+  <si>
+    <t>mm accel path len</t>
+  </si>
+  <si>
+    <t>spindle steps accel path</t>
+  </si>
+  <si>
+    <t>sec, accel time</t>
+  </si>
+  <si>
+    <t>spindle steps when accel</t>
+  </si>
+  <si>
+    <t>mm accel path len by spindle</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="8">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0\ _₽_-;\-* #,##0\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="0.00000000"/>
+    <numFmt numFmtId="175" formatCode="_-* #,##0.0\ _₽_-;\-* #,##0.0\ _₽_-;_-* &quot;-&quot;?\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -267,7 +322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -281,9 +336,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -294,6 +346,13 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -416,6 +475,52 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:yVal>
             <c:numRef>
               <c:f>Лист1!$J$2:$J$35</c:f>
@@ -432,82 +537,82 @@
                   <c:v>660</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0">
-                  <c:v>1063.8297872340424</c:v>
+                  <c:v>1071.4285714285713</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0">
-                  <c:v>1265.8227848101267</c:v>
+                  <c:v>1250</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0">
-                  <c:v>1515.1515151515152</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0">
-                  <c:v>1754.3859649122808</c:v>
+                  <c:v>1764.7058823529412</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0">
                   <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0">
-                  <c:v>2173.913043478261</c:v>
+                  <c:v>2142.8571428571427</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0">
-                  <c:v>2380.9523809523807</c:v>
+                  <c:v>2307.6923076923076</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0">
-                  <c:v>2564.102564102564</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0">
-                  <c:v>2777.7777777777778</c:v>
+                  <c:v>2727.2727272727275</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0">
-                  <c:v>2941.1764705882351</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0">
-                  <c:v>3030.3030303030305</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0">
-                  <c:v>3225.8064516129034</c:v>
+                  <c:v>3333.3333333333335</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0">
                   <c:v>3333.3333333333335</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0">
-                  <c:v>3448.2758620689656</c:v>
+                  <c:v>3333.3333333333335</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0">
-                  <c:v>3571.4285714285716</c:v>
+                  <c:v>3750</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0">
-                  <c:v>3703.7037037037039</c:v>
+                  <c:v>3750</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0">
-                  <c:v>3846.1538461538462</c:v>
+                  <c:v>3750</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0">
-                  <c:v>4000</c:v>
+                  <c:v>3750</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>4166.666666666667</c:v>
+                  <c:v>4285.7142857142853</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0">
-                  <c:v>4166.666666666667</c:v>
+                  <c:v>4285.7142857142853</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0">
-                  <c:v>4347.826086956522</c:v>
+                  <c:v>4285.7142857142853</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0">
-                  <c:v>4347.826086956522</c:v>
+                  <c:v>4285.7142857142853</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0">
-                  <c:v>4545.454545454545</c:v>
+                  <c:v>4285.7142857142853</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0">
-                  <c:v>4545.454545454545</c:v>
+                  <c:v>4285.7142857142853</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0">
-                  <c:v>4761.9047619047615</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0">
-                  <c:v>4761.9047619047615</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0">
                   <c:v>5000</c:v>
@@ -519,10 +624,150 @@
                   <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0">
-                  <c:v>5263.1578947368425</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0">
-                  <c:v>5263.1578947368425</c:v>
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$M$2:$M$35</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #\ ##0.0\ _₽_-;\-* #\ ##0.0\ _₽_-;_-* "-"?\ _₽_-;_-@_-</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1059.4810050208546</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1258.1356436876538</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1504.817494144412</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1752.3148788993626</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1982.5797508212245</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2194.2984959295286</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2389.9003949579878</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2572.0202037980921</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2742.8534492135568</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2904.1375642760904</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3057.2410066734733</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3203.2513579270349</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3343.0442185287829</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3477.3341119711649</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3606.711683246433</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3731.6710136458742</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3852.6298958745169</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3969.9450788590875</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4083.9238834805128</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4194.8331683341985</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4302.9063354782502</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4408.3488678660888</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4511.3427531888328</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4612.0500532348669</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4710.6158103428443</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4807.1704342548719</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4901.8316777630444</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4994.7062839970813</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5085.8913693025606</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5175.475591531047</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5263.5401428956211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -537,11 +782,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="289416224"/>
-        <c:axId val="289417008"/>
+        <c:axId val="374557144"/>
+        <c:axId val="374556360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="289416224"/>
+        <c:axId val="374557144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -597,12 +842,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289417008"/>
+        <c:crossAx val="374556360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="289417008"/>
+        <c:axId val="374556360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,7 +904,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289416224"/>
+        <c:crossAx val="374557144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -891,79 +1136,79 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>250</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>217.39130434782609</c:v>
+                  <c:v>65.217391304347828</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>151.5151515151515</c:v>
+                  <c:v>45.454545454545453</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>94.38583563660174</c:v>
+                  <c:v>28.315750690980522</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55.706562235410821</c:v>
+                  <c:v>16.711968670623246</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>47.754552447166198</c:v>
+                  <c:v>14.326365734149858</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42.744962608104721</c:v>
+                  <c:v>12.823488782431417</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39.15233125065545</c:v>
+                  <c:v>11.745699375196637</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.391558174916732</c:v>
+                  <c:v>10.917467452475021</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.174588334086621</c:v>
+                  <c:v>10.252376500225987</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>32.338609344273529</c:v>
+                  <c:v>9.7015828032820579</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30.782923672557846</c:v>
+                  <c:v>9.2348771017673528</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29.441124783008718</c:v>
+                  <c:v>8.8323374349026142</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28.267252020871918</c:v>
+                  <c:v>8.4801756062615752</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.228268631221315</c:v>
+                  <c:v>8.1684805893663945</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26.299691654173255</c:v>
+                  <c:v>7.8899074962519764</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>25.462914524430218</c:v>
+                  <c:v>7.6388743573290654</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24.703494283588896</c:v>
+                  <c:v>7.411048285076669</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>24.01001579177635</c:v>
+                  <c:v>7.2030047375329058</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>23.373315324226542</c:v>
+                  <c:v>7.0119945972679627</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>22.785935823305138</c:v>
+                  <c:v>6.8357807469915413</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>22.241735943854433</c:v>
+                  <c:v>6.6725207831563296</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>21.735603854384539</c:v>
+                  <c:v>6.5206811563153622</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>21.263244019389543</c:v>
+                  <c:v>6.3789732058168633</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>20.821015851814536</c:v>
+                  <c:v>6.2463047555443607</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1073,82 +1318,82 @@
             <c:numRef>
               <c:f>Лист1!$G$2:$G$26</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>250</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>217.39130434782609</c:v>
+                  <c:v>65.217391304347828</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>151.5151515151515</c:v>
+                  <c:v>45.454545454545453</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>94.38583563660174</c:v>
+                  <c:v>28.315750690980522</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79.48268575151036</c:v>
+                  <c:v>23.84480572545311</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>66.453241266215215</c:v>
+                  <c:v>19.935972379864562</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.067369115081931</c:v>
+                  <c:v>17.120210734524576</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50.439332873534084</c:v>
+                  <c:v>15.131799862060225</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45.572651207436998</c:v>
+                  <c:v>13.671795362231098</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41.842748011997344</c:v>
+                  <c:v>12.552824403599201</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38.87994342047952</c:v>
+                  <c:v>11.663983026143853</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36.458382429681933</c:v>
+                  <c:v>10.937514728904578</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34.43363056561229</c:v>
+                  <c:v>10.330089169683685</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32.709230244431446</c:v>
+                  <c:v>9.8127690733294326</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>31.218280686132108</c:v>
+                  <c:v>9.3654842058396319</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29.912855907125362</c:v>
+                  <c:v>8.9738567721376086</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28.757662272295686</c:v>
+                  <c:v>8.6272986816887069</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>27.726086469431653</c:v>
+                  <c:v>8.317825940829497</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26.797646318317632</c:v>
+                  <c:v>8.0392938954952911</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>25.956295492355036</c:v>
+                  <c:v>7.7868886477065127</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25.189265345892075</c:v>
+                  <c:v>7.5567796037676231</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>24.486254605405446</c:v>
+                  <c:v>7.3458763816216335</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>23.838850315878187</c:v>
+                  <c:v>7.1516550947634556</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23.240106152318887</c:v>
+                  <c:v>6.9720318456956658</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22.68423008190959</c:v>
+                  <c:v>6.8052690245728762</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1261,79 +1506,79 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>250</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>217</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>152</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>94</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>66</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>46</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>39</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>33</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>31</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>30</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>28</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>27</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>26</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>24</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>24</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>23</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1348,11 +1593,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="291385864"/>
-        <c:axId val="291385080"/>
+        <c:axId val="374557928"/>
+        <c:axId val="374558320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="291385864"/>
+        <c:axId val="374557928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1409,12 +1654,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="291385080"/>
+        <c:crossAx val="374558320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="291385080"/>
+        <c:axId val="374558320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1471,7 +1716,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="291385864"/>
+        <c:crossAx val="374557928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1567,14 +1812,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="1.1248906386701742E-3"/>
-          <c:y val="0"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1623,82 +1861,103 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="3"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$N$42:$N$45</c:f>
+              <c:f>Лист1!$R$41:$R$70</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>400</c:v>
+                  <c:v>-400.39677700000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>600</c:v>
+                  <c:v>-395.19657599999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>-384.79639900000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1200</c:v>
+                  <c:v>-369.59624800000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-349.99612500000012</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-326.3960320000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-299.19597100000033</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-268.79594400000019</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-235.59595300000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-199.99600000000009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-162.39608700000031</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-123.19621600000005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-82.79638900000009</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-41.59660800000006</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.1249999997271516E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41.602807999999641</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>82.802438999999595</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>123.20201599999973</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>162.40153699999973</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200.00099999999975</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>235.60040300000037</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>268.79974399999992</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>299.19902099999899</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>326.3982319999991</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>349.99737499999992</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>369.59644799999933</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>384.79544900000019</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>395.19437600000037</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>400.39322699999911</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>399.99199999999973</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1713,11 +1972,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="291384296"/>
-        <c:axId val="291379200"/>
+        <c:axId val="374555968"/>
+        <c:axId val="316336936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="291384296"/>
+        <c:axId val="374555968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1773,12 +2032,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="291379200"/>
+        <c:crossAx val="316336936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="291379200"/>
+        <c:axId val="316336936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1798,7 +2057,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1835,7 +2094,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="291384296"/>
+        <c:crossAx val="374555968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1899,6 +2158,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1937,6 +2197,14 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1947,103 +2215,166 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$R$41:$R$70</c:f>
+              <c:f>Лист1!$M$2:$M$48</c:f>
               <c:numCache>
-                <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:formatCode>_-* #\ ##0.0\ _₽_-;\-* #\ ##0.0\ _₽_-;_-* "-"?\ _₽_-;_-@_-</c:formatCode>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
-                  <c:v>-400.39677700000004</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-395.19657599999994</c:v>
+                  <c:v>460</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-384.79639900000006</c:v>
+                  <c:v>660</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-369.59624800000006</c:v>
+                  <c:v>1059.4810050208546</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-349.99612500000012</c:v>
+                  <c:v>1258.1356436876538</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-326.3960320000001</c:v>
+                  <c:v>1504.817494144412</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-299.19597100000033</c:v>
+                  <c:v>1752.3148788993626</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-268.79594400000019</c:v>
+                  <c:v>1982.5797508212245</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-235.59595300000001</c:v>
+                  <c:v>2194.2984959295286</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-199.99600000000009</c:v>
+                  <c:v>2389.9003949579878</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-162.39608700000031</c:v>
+                  <c:v>2572.0202037980921</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-123.19621600000005</c:v>
+                  <c:v>2742.8534492135568</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-82.79638900000009</c:v>
+                  <c:v>2904.1375642760904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-41.59660800000006</c:v>
+                  <c:v>3057.2410066734733</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.1249999997271516E-3</c:v>
+                  <c:v>3203.2513579270349</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41.602807999999641</c:v>
+                  <c:v>3343.0442185287829</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>82.802438999999595</c:v>
+                  <c:v>3477.3341119711649</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>123.20201599999973</c:v>
+                  <c:v>3606.711683246433</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>162.40153699999973</c:v>
+                  <c:v>3731.6710136458742</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>200.00099999999975</c:v>
+                  <c:v>3852.6298958745169</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>235.60040300000037</c:v>
+                  <c:v>3969.9450788590875</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>268.79974399999992</c:v>
+                  <c:v>4083.9238834805128</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>299.19902099999899</c:v>
+                  <c:v>4194.8331683341985</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>326.3982319999991</c:v>
+                  <c:v>4302.9063354782502</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>349.99737499999992</c:v>
+                  <c:v>4408.3488678660888</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>369.59644799999933</c:v>
+                  <c:v>4511.3427531888328</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>384.79544900000019</c:v>
+                  <c:v>4612.0500532348669</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>395.19437600000037</c:v>
+                  <c:v>4710.6158103428443</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>400.39322699999911</c:v>
+                  <c:v>4807.1704342548719</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>399.99199999999973</c:v>
+                  <c:v>4901.8316777630444</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4994.7062839970813</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5085.8913693025606</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5175.475591531047</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5263.5401428956211</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5350.1595984142568</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5435.4026447106817</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5519.3327090932717</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5602.0085050422858</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5683.4845072507251</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5763.8113669965915</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5843.0362767340303</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5921.2032912717759</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5998.3536116794867</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6074.5258370641368</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6149.756188542643</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>6224.0787090663171</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6297.5254421991112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2058,11 +2389,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="291385472"/>
-        <c:axId val="291379984"/>
+        <c:axId val="374561064"/>
+        <c:axId val="317297144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="291385472"/>
+        <c:axId val="374561064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2118,12 +2449,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="291379984"/>
+        <c:crossAx val="317297144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="291379984"/>
+        <c:axId val="317297144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2143,7 +2474,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:numFmt formatCode="_-* #\ ##0.0\ _₽_-;\-* #\ ##0.0\ _₽_-;_-* &quot;-&quot;?\ _₽_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2180,7 +2511,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="291385472"/>
+        <c:crossAx val="374561064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4457,16 +4788,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>226787</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>426358</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>27214</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>553357</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>70922</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>145143</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>79994</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4487,16 +4818,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>54428</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>166007</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>253997</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>147864</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>371928</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>426355</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>169635</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4517,20 +4848,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>117927</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>84364</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>391138</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>93169</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>380998</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>45357</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>573634</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>34898</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="14" name="Диаграмма 13"/>
+        <xdr:cNvPr id="15" name="Диаграмма 14"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4547,20 +4878,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>291353</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>111312</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>594180</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>175078</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>328706</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>53041</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>303894</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>15421</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="15" name="Диаграмма 14"/>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4576,6 +4907,211 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Лист1"/>
+      <sheetName val="Лист2"/>
+      <sheetName val="Лист3"/>
+      <sheetName val="Лист5"/>
+      <sheetName val="Лист4"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2">
+        <row r="11">
+          <cell r="G11">
+            <v>400</v>
+          </cell>
+          <cell r="L11">
+            <v>3.9215686274509803E-3</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="G12">
+            <v>460.82949308755758</v>
+          </cell>
+          <cell r="L12">
+            <v>3.3333333333333333E-2</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="G13">
+            <v>580</v>
+          </cell>
+          <cell r="L13">
+            <v>4.7619047619047616E-2</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="G14">
+            <v>1063.8297872340424</v>
+          </cell>
+          <cell r="L14">
+            <v>5.8823529411764705E-2</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="G15">
+            <v>1265.8227848101267</v>
+          </cell>
+          <cell r="L15">
+            <v>7.1428571428571425E-2</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="G16">
+            <v>1515.1515151515152</v>
+          </cell>
+          <cell r="L16">
+            <v>8.3333333333333329E-2</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="G17">
+            <v>1900</v>
+          </cell>
+          <cell r="L17">
+            <v>9.0909090909090912E-2</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="G18">
+            <v>2110</v>
+          </cell>
+          <cell r="L18">
+            <v>0.1</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="G19">
+            <v>2173.913043478261</v>
+          </cell>
+          <cell r="L19">
+            <v>0.1111111111111111</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="G20">
+            <v>2380.9523809523807</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="G21">
+            <v>2564.102564102564</v>
+          </cell>
+          <cell r="J21">
+            <v>392.35</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="G22">
+            <v>2777.7777777777778</v>
+          </cell>
+          <cell r="J22">
+            <v>455.81</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="J23">
+            <v>658.83</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="J24">
+            <v>947.8900000000001</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="J25">
+            <v>1274.75</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="J26">
+            <v>1596.4500000000003</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="J27">
+            <v>1875.3100000000004</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="J28">
+            <v>2078.9300000000003</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="J29">
+            <v>2180.1900000000005</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="J30">
+            <v>2157.25</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="J31">
+            <v>1993.5500000000011</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="J32">
+            <v>1677.8100000000031</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="J33">
+            <v>1204.0299999999988</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="J34">
+            <v>571.4900000000016</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="J35">
+            <v>-215.25</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="J36">
+            <v>-1146.3499999999985</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="J37">
+            <v>-2206.6900000000023</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="J38">
+            <v>-3375.8699999999953</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="J39">
+            <v>-4628.2100000000064</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="J40">
+            <v>-5932.75</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4844,7 +5380,7 @@
   <dimension ref="A1:R345"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4852,13 +5388,17 @@
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="15.26953125" customWidth="1"/>
     <col min="3" max="4" width="12.1796875" customWidth="1"/>
-    <col min="9" max="9" width="1.7265625" customWidth="1"/>
+    <col min="8" max="8" width="7.90625" customWidth="1"/>
+    <col min="9" max="9" width="6.36328125" customWidth="1"/>
     <col min="10" max="10" width="6.7265625" customWidth="1"/>
     <col min="11" max="11" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6328125" customWidth="1"/>
+    <col min="13" max="13" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -4868,21 +5408,24 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="20" t="s">
         <v>34</v>
       </c>
       <c r="I1" s="10"/>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4895,24 +5438,33 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="15">
         <f t="shared" ref="F2:F3" si="0">$B$12/J2</f>
-        <v>250</v>
-      </c>
-      <c r="G2" s="3">
+        <v>75</v>
+      </c>
+      <c r="G2" s="21">
         <f>$B$12/J2</f>
-        <v>250</v>
-      </c>
-      <c r="H2" s="13">
+        <v>75</v>
+      </c>
+      <c r="H2" s="12">
         <f>ROUND(G2,0)</f>
-        <v>250</v>
-      </c>
-      <c r="J2" s="15">
+        <v>75</v>
+      </c>
+      <c r="J2" s="14">
         <v>400</v>
       </c>
       <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G2*POWER(2,24),8),",")</f>
+        <v>0x4B000000,</v>
+      </c>
+      <c r="M2" s="19">
+        <f>$B$12/G2</f>
+        <v>400</v>
+      </c>
+      <c r="O2" s="17"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -4924,90 +5476,114 @@
       </c>
       <c r="D3" s="3">
         <f t="shared" ref="D3:D5" si="1">G2-G3</f>
-        <v>32.608695652173907</v>
+        <v>9.7826086956521721</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="15">
         <f t="shared" si="0"/>
-        <v>217.39130434782609</v>
-      </c>
-      <c r="G3" s="3">
+        <v>65.217391304347828</v>
+      </c>
+      <c r="G3" s="21">
         <f>$B$12/J3</f>
-        <v>217.39130434782609</v>
-      </c>
-      <c r="H3" s="14">
+        <v>65.217391304347828</v>
+      </c>
+      <c r="H3" s="13">
         <f>ROUND(G3,0)</f>
-        <v>217</v>
-      </c>
-      <c r="J3" s="15">
+        <v>65</v>
+      </c>
+      <c r="J3" s="14">
         <v>460</v>
       </c>
       <c r="K3" s="4">
         <f t="shared" ref="K3:K5" si="2">J3-J2</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G3*POWER(2,24),8),",")</f>
+        <v>0x4137A6F4,</v>
+      </c>
+      <c r="M3" s="19">
+        <f>$B$12/G3</f>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>
       <c r="D4" s="3">
         <f t="shared" si="1"/>
-        <v>65.876152832674592</v>
+        <v>19.762845849802375</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="15">
         <f>$B$12/J4</f>
-        <v>151.5151515151515</v>
-      </c>
-      <c r="G4" s="3">
+        <v>45.454545454545453</v>
+      </c>
+      <c r="G4" s="21">
         <f>$B$12/J4</f>
-        <v>151.5151515151515</v>
-      </c>
-      <c r="H4" s="14">
+        <v>45.454545454545453</v>
+      </c>
+      <c r="H4" s="13">
         <f>ROUND(G4,0)</f>
-        <v>152</v>
-      </c>
-      <c r="J4" s="15">
+        <v>45</v>
+      </c>
+      <c r="J4" s="14">
         <v>660</v>
       </c>
       <c r="K4" s="4">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G4*POWER(2,24),8),",")</f>
+        <v>0x2D745D17,</v>
+      </c>
+      <c r="M4" s="19">
+        <f>$B$12/G4</f>
+        <v>660</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D5" s="3">
         <f t="shared" si="1"/>
-        <v>57.129315878549761</v>
+        <v>17.138794763564931</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="15">
         <f>B17</f>
-        <v>94.38583563660174</v>
-      </c>
-      <c r="G5" s="3">
+        <v>28.315750690980522</v>
+      </c>
+      <c r="G5" s="21">
         <f>B17</f>
-        <v>94.38583563660174</v>
+        <v>28.315750690980522</v>
       </c>
       <c r="H5" s="8">
         <f>ROUND(G5,0)</f>
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" ref="J5:J35" si="3">$B$12/H5</f>
-        <v>1063.8297872340424</v>
+        <v>1071.4285714285713</v>
       </c>
       <c r="K5" s="4">
         <f t="shared" si="2"/>
-        <v>403.82978723404244</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <v>411.42857142857133</v>
+      </c>
+      <c r="L5" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G5*POWER(2,24),8),",")</f>
+        <v>0x1C50D509,</v>
+      </c>
+      <c r="M5" s="19">
+        <f>$B$12/G5</f>
+        <v>1059.4810050208546</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -5016,113 +5592,137 @@
       </c>
       <c r="D6" s="3">
         <f>G5-G6</f>
-        <v>14.903149885091381</v>
+        <v>4.4709449655274121</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="15">
         <f t="shared" ref="F6:F35" si="4">F5*(1+-1*$B$22*F5*F5)</f>
-        <v>55.706562235410821</v>
-      </c>
-      <c r="G6" s="3">
-        <f t="shared" ref="G6:G35" si="5">G5*(1+I6+1.5*I6*I6)</f>
-        <v>79.48268575151036</v>
+        <v>16.711968670623246</v>
+      </c>
+      <c r="G6" s="21">
+        <f t="shared" ref="G6:G48" si="5">G5*(1+I6+1.5*I6*I6)</f>
+        <v>23.84480572545311</v>
       </c>
       <c r="H6" s="8">
         <f t="shared" ref="H6:H35" si="6">ROUND(G6,0)</f>
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" ref="I6:I35" si="7">-1*$B$22*G5*G5</f>
-        <v>-0.40979955456570155</v>
+        <f t="shared" ref="I6:I48" si="7">-1*$B$22*G5*G5</f>
+        <v>-0.40979955456570161</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="3"/>
-        <v>1265.8227848101267</v>
+        <v>1250</v>
       </c>
       <c r="K6" s="4">
         <f>J6-J5</f>
-        <v>201.99299757608424</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>178.57142857142867</v>
+      </c>
+      <c r="L6" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G6*POWER(2,24),8),",")</f>
+        <v>0x17D84530,</v>
+      </c>
+      <c r="M6" s="19">
+        <f>$B$12/G6</f>
+        <v>1258.1356436876538</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="5">
         <f>((((72000000)/((B6)/(1/B12)))+0.5)-1)</f>
-        <v>719.50000000000011</v>
+        <v>2399.5</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ref="D7:D37" si="8">G6-G7</f>
-        <v>13.029444485295144</v>
+        <v>3.9088333455885476</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="15">
         <f t="shared" si="4"/>
-        <v>47.754552447166198</v>
-      </c>
-      <c r="G7" s="3">
+        <v>14.326365734149858</v>
+      </c>
+      <c r="G7" s="21">
         <f t="shared" si="5"/>
-        <v>66.453241266215215</v>
+        <v>19.935972379864562</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" si="6"/>
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="7"/>
-        <v>-0.29060487737657403</v>
+        <v>-0.29060487737657409</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="3"/>
-        <v>1515.1515151515152</v>
+        <v>1500</v>
       </c>
       <c r="K7" s="4">
         <f t="shared" ref="K7:K35" si="9">J7-J6</f>
-        <v>249.32873034138856</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>250</v>
+      </c>
+      <c r="L7" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G7*POWER(2,24),8),",")</f>
+        <v>0x13EF9BE2,</v>
+      </c>
+      <c r="M7" s="19">
+        <f>$B$12/G7</f>
+        <v>1504.817494144412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="8"/>
-        <v>9.3858721511332845</v>
+        <v>2.8157616453399861</v>
       </c>
       <c r="E8">
         <v>7</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="15">
         <f t="shared" si="4"/>
-        <v>42.744962608104721</v>
-      </c>
-      <c r="G8" s="3">
+        <v>12.823488782431417</v>
+      </c>
+      <c r="G8" s="21">
         <f t="shared" si="5"/>
-        <v>57.067369115081931</v>
+        <v>17.120210734524576</v>
       </c>
       <c r="H8" s="8">
         <f t="shared" si="6"/>
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="7"/>
-        <v>-0.20313753064014722</v>
+        <v>-0.20313753064014717</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="3"/>
-        <v>1754.3859649122808</v>
+        <v>1764.7058823529412</v>
       </c>
       <c r="K8" s="4">
         <f t="shared" si="9"/>
-        <v>239.23444976076553</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>264.70588235294122</v>
+      </c>
+      <c r="L8" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G8*POWER(2,24),8),",")</f>
+        <v>0x111EC621,</v>
+      </c>
+      <c r="M8" s="19">
+        <f>$B$12/G8</f>
+        <v>1752.3148788993626</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -5135,26 +5735,26 @@
       </c>
       <c r="D9" s="3">
         <f t="shared" si="8"/>
-        <v>6.6280362415478464</v>
+        <v>1.9884108724643514</v>
       </c>
       <c r="E9">
         <v>8</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="15">
         <f t="shared" si="4"/>
-        <v>39.15233125065545</v>
-      </c>
-      <c r="G9" s="3">
+        <v>11.745699375196637</v>
+      </c>
+      <c r="G9" s="21">
         <f t="shared" si="5"/>
-        <v>50.439332873534084</v>
+        <v>15.131799862060225</v>
       </c>
       <c r="H9" s="8">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="7"/>
-        <v>-0.14980749241498231</v>
+        <v>-0.14980749241498229</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="3"/>
@@ -5162,10 +5762,18 @@
       </c>
       <c r="K9" s="4">
         <f t="shared" si="9"/>
-        <v>245.61403508771923</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+        <v>235.29411764705878</v>
+      </c>
+      <c r="L9" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G9*POWER(2,24),8),",")</f>
+        <v>0x0F21BDA2,</v>
+      </c>
+      <c r="M9" s="19">
+        <f>$B$12/G9</f>
+        <v>1982.5797508212245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -5178,37 +5786,45 @@
       </c>
       <c r="D10" s="3">
         <f t="shared" si="8"/>
-        <v>4.8666816660970866</v>
+        <v>1.4600044998291271</v>
       </c>
       <c r="E10">
         <v>9</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="15">
         <f t="shared" si="4"/>
-        <v>36.391558174916732</v>
-      </c>
-      <c r="G10" s="3">
+        <v>10.917467452475021</v>
+      </c>
+      <c r="G10" s="21">
         <f t="shared" si="5"/>
-        <v>45.572651207436998</v>
+        <v>13.671795362231098</v>
       </c>
       <c r="H10" s="8">
         <f t="shared" si="6"/>
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" si="7"/>
-        <v>-0.1170298098334501</v>
+        <v>-0.11702980983345011</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="3"/>
-        <v>2173.913043478261</v>
+        <v>2142.8571428571427</v>
       </c>
       <c r="K10" s="4">
         <f t="shared" si="9"/>
-        <v>173.91304347826099</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+        <v>142.85714285714266</v>
+      </c>
+      <c r="L10" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G10*POWER(2,24),8),",")</f>
+        <v>0x0DABFAC7,</v>
+      </c>
+      <c r="M10" s="19">
+        <f>$B$12/G10</f>
+        <v>2194.2984959295286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -5220,151 +5836,183 @@
       </c>
       <c r="D11" s="3">
         <f t="shared" si="8"/>
-        <v>3.729903195439654</v>
+        <v>1.1189709586318966</v>
       </c>
       <c r="E11">
         <v>10</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="15">
         <f t="shared" si="4"/>
-        <v>34.174588334086621</v>
-      </c>
-      <c r="G11" s="3">
+        <v>10.252376500225987</v>
+      </c>
+      <c r="G11" s="21">
         <f t="shared" si="5"/>
-        <v>41.842748011997344</v>
+        <v>12.552824403599201</v>
       </c>
       <c r="H11" s="8">
         <f t="shared" si="6"/>
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" si="7"/>
-        <v>-9.5535860751436608E-2</v>
+        <v>-9.5535860751436594E-2</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="3"/>
-        <v>2380.9523809523807</v>
+        <v>2307.6923076923076</v>
       </c>
       <c r="K11" s="4">
         <f t="shared" si="9"/>
-        <v>207.03933747411975</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+        <v>164.83516483516496</v>
+      </c>
+      <c r="L11" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G11*POWER(2,24),8),",")</f>
+        <v>0x0C8D85E6,</v>
+      </c>
+      <c r="M11" s="19">
+        <f>$B$12/G11</f>
+        <v>2389.9003949579878</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="6">
-        <v>100000</v>
+        <v>30000</v>
       </c>
       <c r="C12" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="8"/>
-        <v>2.9628045915178234</v>
+        <v>0.88884137745534808</v>
       </c>
       <c r="E12">
         <v>11</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="15">
         <f t="shared" si="4"/>
-        <v>32.338609344273529</v>
-      </c>
-      <c r="G12" s="3">
+        <v>9.7015828032820579</v>
+      </c>
+      <c r="G12" s="21">
         <f t="shared" si="5"/>
-        <v>38.87994342047952</v>
+        <v>11.663983026143853</v>
       </c>
       <c r="H12" s="8">
         <f t="shared" si="6"/>
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" si="7"/>
-        <v>-8.0537515814993355E-2</v>
+        <v>-8.0537515814993341E-2</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="3"/>
-        <v>2564.102564102564</v>
+        <v>2500</v>
       </c>
       <c r="K12" s="4">
         <f t="shared" si="9"/>
-        <v>183.15018315018324</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+        <v>192.30769230769238</v>
+      </c>
+      <c r="L12" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G12*POWER(2,24),8),",")</f>
+        <v>0x0BA9FACA,</v>
+      </c>
+      <c r="M12" s="19">
+        <f>$B$12/G12</f>
+        <v>2572.0202037980921</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="8"/>
-        <v>2.4215609907975875</v>
+        <v>0.72646829723927553</v>
       </c>
       <c r="E13">
         <v>12</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="15">
         <f t="shared" si="4"/>
-        <v>30.782923672557846</v>
-      </c>
-      <c r="G13" s="3">
+        <v>9.2348771017673528</v>
+      </c>
+      <c r="G13" s="21">
         <f t="shared" si="5"/>
-        <v>36.458382429681933</v>
+        <v>10.937514728904578</v>
       </c>
       <c r="H13" s="8">
         <f t="shared" si="6"/>
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="7"/>
-        <v>-6.9535900017465679E-2</v>
+        <v>-6.9535900017465652E-2</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="3"/>
-        <v>2777.7777777777778</v>
+        <v>2727.2727272727275</v>
       </c>
       <c r="K13" s="4">
         <f t="shared" si="9"/>
-        <v>213.67521367521385</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+        <v>227.27272727272748</v>
+      </c>
+      <c r="L13" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G13*POWER(2,24),8),",")</f>
+        <v>0x0AF000F7,</v>
+      </c>
+      <c r="M13" s="19">
+        <f>$B$12/G13</f>
+        <v>2742.8534492135568</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="8"/>
-        <v>2.0247518640696427</v>
+        <v>0.60742555922089281</v>
       </c>
       <c r="E14">
         <v>13</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="15">
         <f t="shared" si="4"/>
-        <v>29.441124783008718</v>
-      </c>
-      <c r="G14" s="3">
+        <v>8.8323374349026142</v>
+      </c>
+      <c r="G14" s="21">
         <f t="shared" si="5"/>
-        <v>34.43363056561229</v>
+        <v>10.330089169683685</v>
       </c>
       <c r="H14" s="8">
         <f t="shared" si="6"/>
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="7"/>
-        <v>-6.1143827871891251E-2</v>
+        <v>-6.1143827871891238E-2</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="3"/>
-        <v>2941.1764705882351</v>
+        <v>3000</v>
       </c>
       <c r="K14" s="4">
         <f t="shared" si="9"/>
-        <v>163.39869281045731</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+        <v>272.72727272727252</v>
+      </c>
+      <c r="L14" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G14*POWER(2,24),8),",")</f>
+        <v>0x0A5480B9,</v>
+      </c>
+      <c r="M14" s="19">
+        <f>$B$12/G14</f>
+        <v>2904.1375642760904</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -5374,102 +6022,118 @@
       </c>
       <c r="D15" s="3">
         <f t="shared" si="8"/>
-        <v>1.7244003211808447</v>
+        <v>0.51732009635425236</v>
       </c>
       <c r="E15">
         <v>14</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="15">
         <f t="shared" si="4"/>
-        <v>28.267252020871918</v>
-      </c>
-      <c r="G15" s="3">
+        <v>8.4801756062615752</v>
+      </c>
+      <c r="G15" s="21">
         <f t="shared" si="5"/>
-        <v>32.709230244431446</v>
+        <v>9.8127690733294326</v>
       </c>
       <c r="H15" s="8">
         <f t="shared" si="6"/>
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="I15" s="2">
         <f t="shared" si="7"/>
-        <v>-5.4541046040737173E-2</v>
+        <v>-5.4541046040737153E-2</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="3"/>
-        <v>3030.3030303030305</v>
+        <v>3000</v>
       </c>
       <c r="K15" s="4">
         <f t="shared" si="9"/>
-        <v>89.126559714795349</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="L15" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G15*POWER(2,24),8),",")</f>
+        <v>0x09D011A2,</v>
+      </c>
+      <c r="M15" s="19">
+        <f>$B$12/G15</f>
+        <v>3057.2410066734733</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" si="8"/>
-        <v>1.490949558299338</v>
+        <v>0.44728486748980067</v>
       </c>
       <c r="E16">
         <v>15</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="15">
         <f t="shared" si="4"/>
-        <v>27.228268631221315</v>
-      </c>
-      <c r="G16" s="3">
+        <v>8.1684805893663945</v>
+      </c>
+      <c r="G16" s="21">
         <f t="shared" si="5"/>
-        <v>31.218280686132108</v>
+        <v>9.3654842058396319</v>
       </c>
       <c r="H16" s="8">
         <f t="shared" si="6"/>
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="7"/>
-        <v>-4.9215112186428524E-2</v>
+        <v>-4.9215112186428517E-2</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" si="3"/>
-        <v>3225.8064516129034</v>
+        <v>3333.3333333333335</v>
       </c>
       <c r="K16" s="4">
         <f t="shared" si="9"/>
-        <v>195.50342130987292</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+        <v>333.33333333333348</v>
+      </c>
+      <c r="L16" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G16*POWER(2,24),8),",")</f>
+        <v>0x095D905F,</v>
+      </c>
+      <c r="M16" s="19">
+        <f>$B$12/G16</f>
+        <v>3203.2513579270349</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="3">
         <f>B12/SQRT(B9*B9+2*B11)</f>
-        <v>94.38583563660174</v>
+        <v>28.315750690980522</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="8"/>
-        <v>1.3054247790067457</v>
+        <v>0.39162743370202335</v>
       </c>
       <c r="E17">
         <v>16</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="15">
         <f t="shared" si="4"/>
-        <v>26.299691654173255</v>
-      </c>
-      <c r="G17" s="3">
+        <v>7.8899074962519764</v>
+      </c>
+      <c r="G17" s="21">
         <f t="shared" si="5"/>
-        <v>29.912855907125362</v>
+        <v>8.9738567721376086</v>
       </c>
       <c r="H17" s="8">
         <f t="shared" si="6"/>
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="I17" s="2">
         <f t="shared" si="7"/>
-        <v>-4.4830728253913932E-2</v>
+        <v>-4.4830728253913939E-2</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="3"/>
@@ -5477,324 +6141,396 @@
       </c>
       <c r="K17" s="4">
         <f t="shared" si="9"/>
-        <v>107.52688172043008</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="L17" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G17*POWER(2,24),8),",")</f>
+        <v>0x08F94EAD,</v>
+      </c>
+      <c r="M17" s="19">
+        <f>$B$12/G17</f>
+        <v>3343.0442185287829</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D18" s="3">
         <f t="shared" si="8"/>
-        <v>1.1551936348296756</v>
+        <v>0.34655809044890162</v>
       </c>
       <c r="E18">
         <v>17</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="15">
         <f t="shared" si="4"/>
-        <v>25.462914524430218</v>
-      </c>
-      <c r="G18" s="3">
+        <v>7.6388743573290654</v>
+      </c>
+      <c r="G18" s="21">
         <f t="shared" si="5"/>
-        <v>28.757662272295686</v>
+        <v>8.6272986816887069</v>
       </c>
       <c r="H18" s="8">
         <f t="shared" si="6"/>
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" si="7"/>
-        <v>-4.1159831631940452E-2</v>
+        <v>-4.1159831631940459E-2</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" si="3"/>
-        <v>3448.2758620689656</v>
+        <v>3333.3333333333335</v>
       </c>
       <c r="K18" s="4">
         <f t="shared" si="9"/>
-        <v>114.9425287356321</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="L18" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G18*POWER(2,24),8),",")</f>
+        <v>0x08A096A5,</v>
+      </c>
+      <c r="M18" s="19">
+        <f>$B$12/G18</f>
+        <v>3477.3341119711649</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="3">
         <f t="shared" si="8"/>
-        <v>1.0315758028640332</v>
+        <v>0.30947274085920995</v>
       </c>
       <c r="E19">
         <v>18</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19" s="15">
         <f t="shared" si="4"/>
-        <v>24.703494283588896</v>
-      </c>
-      <c r="G19" s="3">
+        <v>7.411048285076669</v>
+      </c>
+      <c r="G19" s="21">
         <f t="shared" si="5"/>
-        <v>27.726086469431653</v>
+        <v>8.317825940829497</v>
       </c>
       <c r="H19" s="8">
         <f t="shared" si="6"/>
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" si="7"/>
-        <v>-3.8042144410901257E-2</v>
+        <v>-3.8042144410901271E-2</v>
       </c>
       <c r="J19" s="4">
         <f t="shared" si="3"/>
-        <v>3571.4285714285716</v>
+        <v>3750</v>
       </c>
       <c r="K19" s="4">
         <f t="shared" si="9"/>
-        <v>123.15270935960598</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+        <v>416.66666666666652</v>
+      </c>
+      <c r="L19" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G19*POWER(2,24),8),",")</f>
+        <v>0x08515D0A,</v>
+      </c>
+      <c r="M19" s="19">
+        <f>$B$12/G19</f>
+        <v>3606.711683246433</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="3">
         <f>B12/B10</f>
-        <v>16.666666666666668</v>
+        <v>5</v>
       </c>
       <c r="D20" s="3">
         <f t="shared" si="8"/>
-        <v>0.92844015111402101</v>
+        <v>0.27853204533420595</v>
       </c>
       <c r="E20">
         <v>19</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="15">
         <f t="shared" si="4"/>
-        <v>24.01001579177635</v>
-      </c>
-      <c r="G20" s="3">
+        <v>7.2030047375329058</v>
+      </c>
+      <c r="G20" s="21">
         <f t="shared" si="5"/>
-        <v>26.797646318317632</v>
+        <v>8.0392938954952911</v>
       </c>
       <c r="H20" s="8">
         <f t="shared" si="6"/>
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" si="7"/>
-        <v>-3.5361850061878447E-2</v>
+        <v>-3.5361850061878461E-2</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" si="3"/>
-        <v>3703.7037037037039</v>
+        <v>3750</v>
       </c>
       <c r="K20" s="4">
         <f t="shared" si="9"/>
-        <v>132.27513227513236</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="L20" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G20*POWER(2,24),8),",")</f>
+        <v>0x080A0F2A,</v>
+      </c>
+      <c r="M20" s="19">
+        <f>$B$12/G20</f>
+        <v>3731.6710136458742</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="3">
         <f t="shared" si="8"/>
-        <v>0.84135082596259636</v>
+        <v>0.25240524778877838</v>
       </c>
       <c r="E21">
         <v>20</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21" s="15">
         <f t="shared" si="4"/>
-        <v>23.373315324226542</v>
-      </c>
-      <c r="G21" s="3">
+        <v>7.0119945972679627</v>
+      </c>
+      <c r="G21" s="21">
         <f t="shared" si="5"/>
-        <v>25.956295492355036</v>
+        <v>7.7868886477065127</v>
       </c>
       <c r="H21" s="8">
         <f t="shared" si="6"/>
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="I21" s="2">
         <f t="shared" si="7"/>
-        <v>-3.3033237017275556E-2</v>
+        <v>-3.3033237017275577E-2</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" si="3"/>
-        <v>3846.1538461538462</v>
+        <v>3750</v>
       </c>
       <c r="K21" s="4">
         <f t="shared" si="9"/>
-        <v>142.45014245014227</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="L21" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G21*POWER(2,24),8),",")</f>
+        <v>0x07C97188,</v>
+      </c>
+      <c r="M21" s="19">
+        <f>$B$12/G21</f>
+        <v>3852.6298958745169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>26</v>
       </c>
       <c r="B22">
         <f>B11/(B12*B12)</f>
-        <v>4.6E-5</v>
+        <v>5.1111111111111116E-4</v>
       </c>
       <c r="D22" s="3">
         <f t="shared" si="8"/>
-        <v>0.76703014646296097</v>
+        <v>0.23010904393888953</v>
       </c>
       <c r="E22">
         <v>21</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="15">
         <f t="shared" si="4"/>
-        <v>22.785935823305138</v>
-      </c>
-      <c r="G22" s="3">
+        <v>6.8357807469915413</v>
+      </c>
+      <c r="G22" s="21">
         <f t="shared" si="5"/>
-        <v>25.189265345892075</v>
+        <v>7.5567796037676231</v>
       </c>
       <c r="H22" s="8">
         <f t="shared" si="6"/>
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" si="7"/>
-        <v>-3.0991546681576713E-2</v>
+        <v>-3.0991546681576734E-2</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" si="3"/>
-        <v>4000</v>
+        <v>3750</v>
       </c>
       <c r="K22" s="4">
         <f t="shared" si="9"/>
-        <v>153.84615384615381</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="L22" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G22*POWER(2,24),8),",")</f>
+        <v>0x078E891B,</v>
+      </c>
+      <c r="M22" s="19">
+        <f>$B$12/G22</f>
+        <v>3969.9450788590875</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="3">
         <f t="shared" si="8"/>
-        <v>0.70301074048662926</v>
+        <v>0.21090322214598967</v>
       </c>
       <c r="E23">
         <v>22</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F23" s="15">
         <f t="shared" si="4"/>
-        <v>22.241735943854433</v>
-      </c>
-      <c r="G23" s="3">
+        <v>6.6725207831563296</v>
+      </c>
+      <c r="G23" s="21">
         <f t="shared" si="5"/>
-        <v>24.486254605405446</v>
+        <v>7.3458763816216335</v>
       </c>
       <c r="H23" s="8">
         <f t="shared" si="6"/>
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="I23" s="2">
         <f t="shared" si="7"/>
-        <v>-2.9186958078624932E-2</v>
+        <v>-2.9186958078624939E-2</v>
       </c>
       <c r="J23" s="4">
         <f t="shared" si="3"/>
-        <v>4166.666666666667</v>
+        <v>4285.7142857142853</v>
       </c>
       <c r="K23" s="4">
         <f t="shared" si="9"/>
-        <v>166.66666666666697</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+        <v>535.71428571428532</v>
+      </c>
+      <c r="L23" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G23*POWER(2,24),8),",")</f>
+        <v>0x07588B5A,</v>
+      </c>
+      <c r="M23" s="19">
+        <f>$B$12/G23</f>
+        <v>4083.9238834805128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="3">
         <f t="shared" si="8"/>
-        <v>0.64740428952725892</v>
+        <v>0.19422128685817786</v>
       </c>
       <c r="E24">
         <v>23</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="15">
         <f t="shared" si="4"/>
-        <v>21.735603854384539</v>
-      </c>
-      <c r="G24" s="3">
+        <v>6.5206811563153622</v>
+      </c>
+      <c r="G24" s="21">
         <f t="shared" si="5"/>
-        <v>23.838850315878187</v>
+        <v>7.1516550947634556</v>
       </c>
       <c r="H24" s="8">
         <f t="shared" si="6"/>
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="I24" s="2">
         <f t="shared" si="7"/>
-        <v>-2.7580526571634009E-2</v>
+        <v>-2.7580526571634015E-2</v>
       </c>
       <c r="J24" s="4">
         <f t="shared" si="3"/>
-        <v>4166.666666666667</v>
+        <v>4285.7142857142853</v>
       </c>
       <c r="K24" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L24" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G24*POWER(2,24),8),",")</f>
+        <v>0x0726D2DE,</v>
+      </c>
+      <c r="M24" s="19">
+        <f>$B$12/G24</f>
+        <v>4194.8331683341985</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="D25" s="3">
         <f t="shared" si="8"/>
-        <v>0.59874416355929938</v>
+        <v>0.17962324906778981</v>
       </c>
       <c r="E25">
         <v>24</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F25" s="15">
         <f t="shared" si="4"/>
-        <v>21.263244019389543</v>
-      </c>
-      <c r="G25" s="3">
+        <v>6.3789732058168633</v>
+      </c>
+      <c r="G25" s="21">
         <f t="shared" si="5"/>
-        <v>23.240106152318887</v>
+        <v>6.9720318456956658</v>
       </c>
       <c r="H25" s="8">
         <f t="shared" si="6"/>
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="I25" s="2">
         <f t="shared" si="7"/>
-        <v>-2.6141376081610896E-2</v>
+        <v>-2.6141376081610893E-2</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" si="3"/>
-        <v>4347.826086956522</v>
+        <v>4285.7142857142853</v>
       </c>
       <c r="K25" s="4">
         <f t="shared" si="9"/>
-        <v>181.15942028985501</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="L25" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G25*POWER(2,24),8),",")</f>
+        <v>0x06F8D714,</v>
+      </c>
+      <c r="M25" s="19">
+        <f>$B$12/G25</f>
+        <v>4302.9063354782502</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>16</v>
       </c>
       <c r="D26" s="3">
         <f t="shared" si="8"/>
-        <v>0.55587607040929754</v>
+        <v>0.16676282112278962</v>
       </c>
       <c r="E26">
         <v>25</v>
       </c>
-      <c r="F26" s="16">
+      <c r="F26" s="15">
         <f t="shared" si="4"/>
-        <v>20.821015851814536</v>
-      </c>
-      <c r="G26" s="3">
+        <v>6.2463047555443607</v>
+      </c>
+      <c r="G26" s="21">
         <f t="shared" si="5"/>
-        <v>22.68423008190959</v>
+        <v>6.8052690245728762</v>
       </c>
       <c r="H26" s="8">
         <f t="shared" si="6"/>
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="I26" s="2">
         <f t="shared" si="7"/>
@@ -5802,183 +6538,223 @@
       </c>
       <c r="J26" s="4">
         <f t="shared" si="3"/>
-        <v>4347.826086956522</v>
+        <v>4285.7142857142853</v>
       </c>
       <c r="K26" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L26" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G26*POWER(2,24),8),",")</f>
+        <v>0x06CE261C,</v>
+      </c>
+      <c r="M26" s="19">
+        <f>$B$12/G26</f>
+        <v>4408.3488678660888</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>17</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" si="8"/>
-        <v>0.51788062213616826</v>
+        <v>0.15536418664085083</v>
       </c>
       <c r="E27">
         <v>26</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="15">
         <f t="shared" si="4"/>
-        <v>20.405809894487593</v>
-      </c>
-      <c r="G27" s="3">
+        <v>6.1217429683462772</v>
+      </c>
+      <c r="G27" s="21">
         <f t="shared" si="5"/>
-        <v>22.166349459773421</v>
+        <v>6.6499048379320254</v>
       </c>
       <c r="H27" s="8">
         <f t="shared" si="6"/>
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="I27" s="2">
         <f t="shared" si="7"/>
-        <v>-2.3670417542814549E-2</v>
+        <v>-2.3670417542814546E-2</v>
       </c>
       <c r="J27" s="4">
         <f t="shared" si="3"/>
-        <v>4545.454545454545</v>
+        <v>4285.7142857142853</v>
       </c>
       <c r="K27" s="4">
         <f t="shared" si="9"/>
-        <v>197.62845849802306</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="L27" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G27*POWER(2,24),8),",")</f>
+        <v>0x06A66029,</v>
+      </c>
+      <c r="M27" s="19">
+        <f>$B$12/G27</f>
+        <v>4511.3427531888328</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>18</v>
       </c>
       <c r="D28" s="3">
         <f t="shared" si="8"/>
-        <v>0.48401755839681826</v>
+        <v>0.14520526751904494</v>
       </c>
       <c r="E28">
         <v>27</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="15">
         <f t="shared" si="4"/>
-        <v>20.014951592746637</v>
-      </c>
-      <c r="G28" s="3">
+        <v>6.00448547782399</v>
+      </c>
+      <c r="G28" s="21">
         <f t="shared" si="5"/>
-        <v>21.682331901376603</v>
+        <v>6.5046995704129804</v>
       </c>
       <c r="H28" s="8">
         <f t="shared" si="6"/>
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="I28" s="2">
         <f t="shared" si="7"/>
-        <v>-2.2601964225148683E-2</v>
+        <v>-2.260196422514868E-2</v>
       </c>
       <c r="J28" s="4">
         <f t="shared" si="3"/>
-        <v>4545.454545454545</v>
+        <v>4285.7142857142853</v>
       </c>
       <c r="K28" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L28" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G28*POWER(2,24),8),",")</f>
+        <v>0x068133FD,</v>
+      </c>
+      <c r="M28" s="19">
+        <f>$B$12/G28</f>
+        <v>4612.0500532348669</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" si="8"/>
-        <v>0.45368494179322738</v>
+        <v>0.1361054825379675</v>
       </c>
       <c r="E29">
         <v>28</v>
       </c>
-      <c r="F29" s="16">
+      <c r="F29" s="15">
         <f t="shared" si="4"/>
-        <v>19.646125647674925</v>
-      </c>
-      <c r="G29" s="3">
+        <v>5.8938376943024755</v>
+      </c>
+      <c r="G29" s="21">
         <f t="shared" si="5"/>
-        <v>21.228646959583376</v>
+        <v>6.3685940878750129</v>
       </c>
       <c r="H29" s="8">
         <f t="shared" si="6"/>
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="I29" s="2">
         <f t="shared" si="7"/>
-        <v>-2.1625681767346864E-2</v>
+        <v>-2.162568176734686E-2</v>
       </c>
       <c r="J29" s="4">
         <f t="shared" si="3"/>
-        <v>4761.9047619047615</v>
+        <v>5000</v>
       </c>
       <c r="K29" s="4">
         <f t="shared" si="9"/>
-        <v>216.45021645021643</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+        <v>714.28571428571468</v>
+      </c>
+      <c r="L29" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G29*POWER(2,24),8),",")</f>
+        <v>0x065E5C2E,</v>
+      </c>
+      <c r="M29" s="19">
+        <f>$B$12/G29</f>
+        <v>4710.6158103428443</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="3">
         <f t="shared" si="8"/>
-        <v>0.42638888122998253</v>
+        <v>0.1279166643689944</v>
       </c>
       <c r="E30">
         <v>29</v>
       </c>
-      <c r="F30" s="16">
+      <c r="F30" s="15">
         <f t="shared" si="4"/>
-        <v>19.297315923718919</v>
-      </c>
-      <c r="G30" s="3">
+        <v>5.7891947771156733</v>
+      </c>
+      <c r="G30" s="21">
         <f t="shared" si="5"/>
-        <v>20.802258078353393</v>
+        <v>6.2406774235060185</v>
       </c>
       <c r="H30" s="8">
         <f t="shared" si="6"/>
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="I30" s="2">
         <f t="shared" si="7"/>
-        <v>-2.073015077979291E-2</v>
+        <v>-2.0730150779792914E-2</v>
       </c>
       <c r="J30" s="4">
         <f t="shared" si="3"/>
-        <v>4761.9047619047615</v>
+        <v>5000</v>
       </c>
       <c r="K30" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L30" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G30*POWER(2,24),8),",")</f>
+        <v>0x063D9D09,</v>
+      </c>
+      <c r="M30" s="19">
+        <f>$B$12/G30</f>
+        <v>4807.1704342548719</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="3">
         <f t="shared" si="8"/>
-        <v>0.40172077438071341</v>
+        <v>0.12051623231421349</v>
       </c>
       <c r="E31">
         <v>30</v>
       </c>
-      <c r="F31" s="16">
+      <c r="F31" s="15">
         <f t="shared" si="4"/>
-        <v>18.96675725376917</v>
-      </c>
-      <c r="G31" s="3">
+        <v>5.6900271761307488</v>
+      </c>
+      <c r="G31" s="21">
         <f t="shared" si="5"/>
-        <v>20.40053730397268</v>
+        <v>6.120161191191805</v>
       </c>
       <c r="H31" s="8">
         <f t="shared" si="6"/>
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" si="7"/>
-        <v>-1.9905761293287274E-2</v>
+        <v>-1.9905761293287281E-2</v>
       </c>
       <c r="J31" s="4">
         <f t="shared" si="3"/>
@@ -5986,35 +6762,43 @@
       </c>
       <c r="K31" s="4">
         <f t="shared" si="9"/>
-        <v>238.09523809523853</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="L31" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G31*POWER(2,24),8),",")</f>
+        <v>0x061EC2E2,</v>
+      </c>
+      <c r="M31" s="19">
+        <f>$B$12/G31</f>
+        <v>4901.8316777630444</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>22</v>
       </c>
       <c r="D32" s="3">
         <f t="shared" si="8"/>
-        <v>0.3793399974568672</v>
+        <v>0.1138019992370598</v>
       </c>
       <c r="E32">
         <v>31</v>
       </c>
-      <c r="F32" s="16">
+      <c r="F32" s="15">
         <f t="shared" si="4"/>
-        <v>18.652896445070525</v>
-      </c>
-      <c r="G32" s="3">
+        <v>5.5958689335211558</v>
+      </c>
+      <c r="G32" s="21">
         <f t="shared" si="5"/>
-        <v>20.021197306515813</v>
+        <v>6.0063591919547452</v>
       </c>
       <c r="H32" s="8">
         <f t="shared" si="6"/>
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="I32" s="2">
         <f t="shared" si="7"/>
-        <v>-1.914436842537592E-2</v>
+        <v>-1.9144368425375931E-2</v>
       </c>
       <c r="J32" s="4">
         <f t="shared" si="3"/>
@@ -6024,6 +6808,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="L32" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G32*POWER(2,24),8),",")</f>
+        <v>0x0601A0C1,</v>
+      </c>
+      <c r="M32" s="19">
+        <f>$B$12/G32</f>
+        <v>4994.7062839970813</v>
+      </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
@@ -6031,26 +6823,26 @@
       </c>
       <c r="D33" s="3">
         <f t="shared" si="8"/>
-        <v>0.35896059348251441</v>
+        <v>0.10768817804475539</v>
       </c>
       <c r="E33">
         <v>32</v>
       </c>
-      <c r="F33" s="16">
+      <c r="F33" s="15">
         <f t="shared" si="4"/>
-        <v>18.354360472797978</v>
-      </c>
-      <c r="G33" s="3">
+        <v>5.5063081418393915</v>
+      </c>
+      <c r="G33" s="21">
         <f t="shared" si="5"/>
-        <v>19.662236713033298</v>
+        <v>5.8986710139099898</v>
       </c>
       <c r="H33" s="8">
         <f t="shared" si="6"/>
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="I33" s="2">
         <f t="shared" si="7"/>
-        <v>-1.8439023712976059E-2</v>
+        <v>-1.8439023712976066E-2</v>
       </c>
       <c r="J33" s="4">
         <f t="shared" si="3"/>
@@ -6060,38 +6852,54 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="L33" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G33*POWER(2,24),8),",")</f>
+        <v>0x05E60F4D,</v>
+      </c>
+      <c r="M33" s="19">
+        <f>$B$12/G33</f>
+        <v>5085.8913693025606</v>
+      </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="D34" s="3">
         <f t="shared" si="8"/>
-        <v>0.3403409313903083</v>
+        <v>0.10210227941709249</v>
       </c>
       <c r="E34">
         <v>33</v>
       </c>
-      <c r="F34" s="16">
+      <c r="F34" s="15">
         <f t="shared" si="4"/>
-        <v>18.069930341232077</v>
+        <v>5.4209791023696212</v>
       </c>
       <c r="G34" s="3">
         <f t="shared" si="5"/>
-        <v>19.32189578164299</v>
+        <v>5.7965687344928973</v>
       </c>
       <c r="H34" s="8">
         <f t="shared" si="6"/>
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="I34" s="2">
         <f t="shared" si="7"/>
-        <v>-1.7783763417730306E-2</v>
+        <v>-1.778376341773031E-2</v>
       </c>
       <c r="J34" s="4">
         <f t="shared" si="3"/>
-        <v>5263.1578947368425</v>
+        <v>5000</v>
       </c>
       <c r="K34" s="4">
         <f t="shared" si="9"/>
-        <v>263.15789473684254</v>
+        <v>0</v>
+      </c>
+      <c r="L34" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G34*POWER(2,24),8),",")</f>
+        <v>0x05CBEBED,</v>
+      </c>
+      <c r="M34" s="19">
+        <f>$B$12/G34</f>
+        <v>5175.475591531047</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6100,35 +6908,43 @@
       </c>
       <c r="D35" s="3">
         <f t="shared" si="8"/>
-        <v>0.32327559728410193</v>
+        <v>9.6982679185231291E-2</v>
       </c>
       <c r="E35">
         <v>34</v>
       </c>
-      <c r="F35" s="16">
+      <c r="F35" s="15">
         <f t="shared" si="4"/>
-        <v>17.798519452696446</v>
+        <v>5.3395558358089321</v>
       </c>
       <c r="G35" s="3">
         <f t="shared" si="5"/>
-        <v>18.998620184358888</v>
+        <v>5.699586055307666</v>
       </c>
       <c r="H35" s="9">
         <f t="shared" si="6"/>
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="I35" s="2">
         <f t="shared" si="7"/>
-        <v>-1.7173440203446966E-2</v>
+        <v>-1.7173440203446969E-2</v>
       </c>
       <c r="J35" s="4">
         <f t="shared" si="3"/>
-        <v>5263.1578947368425</v>
+        <v>5000</v>
       </c>
       <c r="K35" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="L35" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G35*POWER(2,24),8),",")</f>
+        <v>0x05B31812,</v>
+      </c>
+      <c r="M35" s="19">
+        <f>$B$12/G35</f>
+        <v>5263.5401428956211</v>
+      </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -6136,7 +6952,23 @@
       </c>
       <c r="D36" s="3">
         <f t="shared" si="8"/>
-        <v>18.998620184358888</v>
+        <v>9.2276694126786296E-2</v>
+      </c>
+      <c r="G36" s="3">
+        <f t="shared" si="5"/>
+        <v>5.6073093611808797</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.660358816983833E-2</v>
+      </c>
+      <c r="L36" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G36*POWER(2,24),8),",")</f>
+        <v>0x059B78A0,</v>
+      </c>
+      <c r="M36" s="19">
+        <f>$B$12/G36</f>
+        <v>5350.1595984142568</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.35">
@@ -6145,14 +6977,100 @@
       </c>
       <c r="D37" s="3">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.7939047521834013E-2</v>
+      </c>
+      <c r="G37" s="3">
+        <f t="shared" si="5"/>
+        <v>5.5193703136590457</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.6070313783459883E-2</v>
+      </c>
+      <c r="L37" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G37*POWER(2,24),8),",")</f>
+        <v>0x0584F573,</v>
+      </c>
+      <c r="M37" s="19">
+        <f>$B$12/G37</f>
+        <v>5435.4026447106817</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G38" s="3">
+        <f t="shared" si="5"/>
+        <v>5.4354396774403675</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.5570207092531499E-2</v>
+      </c>
+      <c r="L38" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G38*POWER(2,24),8),",")</f>
+        <v>0x056F78F9,</v>
+      </c>
+      <c r="M38" s="19">
+        <f>$B$12/G38</f>
+        <v>5519.3327090932717</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G39" s="3">
+        <f t="shared" si="5"/>
+        <v>5.3552221445214583</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.5100268960069779E-2</v>
+      </c>
+      <c r="L39" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G39*POWER(2,24),8),",")</f>
+        <v>0x055AEFD6,</v>
+      </c>
+      <c r="M39" s="19">
+        <f>$B$12/G39</f>
+        <v>5602.0085050422858</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G40" s="3">
+        <f t="shared" si="5"/>
+        <v>5.2784519710975539</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.4657851044332872E-2</v>
+      </c>
+      <c r="L40" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G40*POWER(2,24),8),",")</f>
+        <v>0x054748A0,</v>
+      </c>
+      <c r="M40" s="19">
+        <f>$B$12/G40</f>
+        <v>5683.4845072507251</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G41" s="3">
+        <f t="shared" si="5"/>
+        <v>5.204889280690046</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.4240605996827201E-2</v>
+      </c>
+      <c r="L41" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G41*POWER(2,24),8),",")</f>
+        <v>0x0534739F,</v>
+      </c>
+      <c r="M41" s="19">
+        <f>$B$12/G41</f>
+        <v>5763.8113669965915</v>
+      </c>
       <c r="Q41">
         <v>1.1000000000000001</v>
       </c>
-      <c r="R41" s="17">
+      <c r="R41" s="16">
         <f xml:space="preserve"> -66.667*POWER(Q41,3) + 500*POWER(Q41,2) - 833.33*Q41</f>
         <v>-400.39677700000004</v>
       </c>
@@ -6160,18 +7078,26 @@
     <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
-      <c r="I42" s="2"/>
-      <c r="M42">
-        <v>200</v>
-      </c>
-      <c r="N42">
-        <f>M42+200</f>
-        <v>400</v>
+      <c r="G42" s="3">
+        <f t="shared" si="5"/>
+        <v>5.1343169166097535</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.3846445905723764E-2</v>
+      </c>
+      <c r="L42" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G42*POWER(2,24),8),",")</f>
+        <v>0x05226297,</v>
+      </c>
+      <c r="M42" s="19">
+        <f>$B$12/G42</f>
+        <v>5843.0362767340303</v>
       </c>
       <c r="Q42">
         <v>1.2</v>
       </c>
-      <c r="R42" s="17">
+      <c r="R42" s="16">
         <f t="shared" ref="R42:R70" si="10" xml:space="preserve"> -66.667*POWER(Q42,3) + 500*POWER(Q42,2) - 833.33*Q42</f>
         <v>-395.19657599999994</v>
       </c>
@@ -6179,18 +7105,26 @@
     <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-      <c r="I43" s="2"/>
-      <c r="M43">
-        <v>400</v>
-      </c>
-      <c r="N43">
-        <f t="shared" ref="N43:N45" si="11">M43+200</f>
-        <v>600</v>
+      <c r="G43" s="3">
+        <f t="shared" si="5"/>
+        <v>5.0665377498897692</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.3473507435650156E-2</v>
+      </c>
+      <c r="L43" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G43*POWER(2,24),8),",")</f>
+        <v>0x0511089E,</v>
+      </c>
+      <c r="M43" s="19">
+        <f>$B$12/G43</f>
+        <v>5921.2032912717759</v>
       </c>
       <c r="Q43">
         <v>1.3</v>
       </c>
-      <c r="R43" s="17">
+      <c r="R43" s="16">
         <f t="shared" si="10"/>
         <v>-384.79639900000006</v>
       </c>
@@ -6198,18 +7132,26 @@
     <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
-      <c r="I44" s="2"/>
-      <c r="M44">
-        <v>800</v>
-      </c>
-      <c r="N44">
-        <f t="shared" si="11"/>
-        <v>1000</v>
+      <c r="G44" s="3">
+        <f t="shared" si="5"/>
+        <v>5.0013723668418848</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.3120122438540801E-2</v>
+      </c>
+      <c r="L44" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G44*POWER(2,24),8),",")</f>
+        <v>0x050059F0,</v>
+      </c>
+      <c r="M44" s="19">
+        <f>$B$12/G44</f>
+        <v>5998.3536116794867</v>
       </c>
       <c r="Q44">
         <v>1.4</v>
       </c>
-      <c r="R44" s="17">
+      <c r="R44" s="16">
         <f t="shared" si="10"/>
         <v>-369.59624800000006</v>
       </c>
@@ -6217,18 +7159,26 @@
     <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
-      <c r="I45" s="2"/>
-      <c r="M45">
-        <v>1000</v>
-      </c>
-      <c r="N45">
-        <f t="shared" si="11"/>
-        <v>1200</v>
+      <c r="G45" s="3">
+        <f t="shared" si="5"/>
+        <v>4.9386570745905694</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.2784793059813795E-2</v>
+      </c>
+      <c r="L45" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G45*POWER(2,24),8),",")</f>
+        <v>0x04F04BD4,</v>
+      </c>
+      <c r="M45" s="19">
+        <f>$B$12/G45</f>
+        <v>6074.5258370641368</v>
       </c>
       <c r="Q45">
         <v>1.5</v>
       </c>
-      <c r="R45" s="17">
+      <c r="R45" s="16">
         <f t="shared" si="10"/>
         <v>-349.99612500000012</v>
       </c>
@@ -6236,11 +7186,26 @@
     <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-      <c r="I46" s="2"/>
+      <c r="G46" s="3">
+        <f t="shared" si="5"/>
+        <v>4.878242174200623</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.2466170557984003E-2</v>
+      </c>
+      <c r="L46" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G46*POWER(2,24),8),",")</f>
+        <v>0x04E0D47A,</v>
+      </c>
+      <c r="M46" s="19">
+        <f>$B$12/G46</f>
+        <v>6149.756188542643</v>
+      </c>
       <c r="Q46">
         <v>1.6</v>
       </c>
-      <c r="R46" s="17">
+      <c r="R46" s="16">
         <f t="shared" si="10"/>
         <v>-326.3960320000001</v>
       </c>
@@ -6248,11 +7213,26 @@
     <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
-      <c r="I47" s="2"/>
+      <c r="G47" s="3">
+        <f t="shared" si="5"/>
+        <v>4.8199904600018053</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.2163037207409808E-2</v>
+      </c>
+      <c r="L47" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G47*POWER(2,24),8),",")</f>
+        <v>0x04D1EAE5,</v>
+      </c>
+      <c r="M47" s="19">
+        <f>$B$12/G47</f>
+        <v>6224.0787090663171</v>
+      </c>
       <c r="Q47">
         <v>1.7</v>
       </c>
-      <c r="R47" s="17">
+      <c r="R47" s="16">
         <f t="shared" si="10"/>
         <v>-299.19597100000033</v>
       </c>
@@ -6260,11 +7240,26 @@
     <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
-      <c r="I48" s="2"/>
+      <c r="G48" s="3">
+        <f t="shared" si="5"/>
+        <v>4.763775910927313</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.1874290773193191E-2</v>
+      </c>
+      <c r="L48" t="str">
+        <f>CONCATENATE("0x",DEC2HEX(G48*POWER(2,24),8),",")</f>
+        <v>0x04C386D1,</v>
+      </c>
+      <c r="M48" s="19">
+        <f>$B$12/G48</f>
+        <v>6297.5254421991112</v>
+      </c>
       <c r="Q48">
         <v>1.8</v>
       </c>
-      <c r="R48" s="17">
+      <c r="R48" s="16">
         <f t="shared" si="10"/>
         <v>-268.79594400000019</v>
       </c>
@@ -6272,11 +7267,26 @@
     <row r="49" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
-      <c r="I49" s="2"/>
+      <c r="G49" s="3">
+        <f t="shared" ref="G49:G53" si="11">G48*(1+I49+1.5*I49*I49)</f>
+        <v>4.7094825455050353</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" ref="I49:I53" si="12">-1*$B$22*G48*G48</f>
+        <v>-1.159893114176047E-2</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" ref="L49:L53" si="13">CONCATENATE("0x",DEC2HEX(G49*POWER(2,24),8),",")</f>
+        <v>0x04B5A0A5,</v>
+      </c>
+      <c r="M49" s="19">
+        <f t="shared" ref="M49:M53" si="14">$B$12/G49</f>
+        <v>6370.12659249231</v>
+      </c>
       <c r="Q49">
         <v>1.9</v>
       </c>
-      <c r="R49" s="17">
+      <c r="R49" s="16">
         <f t="shared" si="10"/>
         <v>-235.59595300000001</v>
       </c>
@@ -6284,11 +7294,26 @@
     <row r="50" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
-      <c r="I50" s="2"/>
+      <c r="G50" s="3">
+        <f t="shared" si="11"/>
+        <v>4.6570034168642778</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="12"/>
+        <v>-1.1336048765946257E-2</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="13"/>
+        <v>0x04A83160,</v>
+      </c>
+      <c r="M50" s="19">
+        <f t="shared" si="14"/>
+        <v>6441.9106697156003</v>
+      </c>
       <c r="Q50">
         <v>2</v>
       </c>
-      <c r="R50" s="17">
+      <c r="R50" s="16">
         <f t="shared" si="10"/>
         <v>-199.99600000000009</v>
       </c>
@@ -6296,11 +7321,26 @@
     <row r="51" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
-      <c r="I51" s="2"/>
+      <c r="G51" s="3">
+        <f t="shared" si="11"/>
+        <v>4.6062397279725129</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="12"/>
+        <v>-1.1084814643728175E-2</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="13"/>
+        <v>0x049B3286,</v>
+      </c>
+      <c r="M51" s="19">
+        <f t="shared" si="14"/>
+        <v>6512.9046188841821</v>
+      </c>
       <c r="Q51">
         <v>2.1</v>
       </c>
-      <c r="R51" s="17">
+      <c r="R51" s="16">
         <f t="shared" si="10"/>
         <v>-162.39608700000031</v>
       </c>
@@ -6308,11 +7348,26 @@
     <row r="52" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
-      <c r="I52" s="2"/>
+      <c r="G52" s="3">
+        <f t="shared" si="11"/>
+        <v>4.5571000504726502</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="12"/>
+        <v>-1.0844471598348948E-2</v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="13"/>
+        <v>0x048E9E1B,</v>
+      </c>
+      <c r="M52" s="19">
+        <f t="shared" si="14"/>
+        <v>6583.133937752471</v>
+      </c>
       <c r="Q52">
         <v>2.2000000000000002</v>
       </c>
-      <c r="R52" s="17">
+      <c r="R52" s="16">
         <f t="shared" si="10"/>
         <v>-123.19621600000005</v>
       </c>
@@ -6320,11 +7375,26 @@
     <row r="53" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
-      <c r="I53" s="2"/>
+      <c r="G53" s="3">
+        <f t="shared" si="11"/>
+        <v>4.5094996330888746</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="12"/>
+        <v>-1.0614326666898004E-2</v>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="13"/>
+        <v>0x04826E91,</v>
+      </c>
+      <c r="M53" s="19">
+        <f t="shared" si="14"/>
+        <v>6652.6227832179429</v>
+      </c>
       <c r="Q53">
         <v>2.2999999999999998</v>
       </c>
-      <c r="R53" s="17">
+      <c r="R53" s="16">
         <f t="shared" si="10"/>
         <v>-82.79638900000009</v>
       </c>
@@ -6336,7 +7406,7 @@
       <c r="Q54">
         <v>2.4</v>
       </c>
-      <c r="R54" s="17">
+      <c r="R54" s="16">
         <f t="shared" si="10"/>
         <v>-41.59660800000006</v>
       </c>
@@ -6348,7 +7418,7 @@
       <c r="Q55">
         <v>2.5</v>
       </c>
-      <c r="R55" s="17">
+      <c r="R55" s="16">
         <f t="shared" si="10"/>
         <v>3.1249999997271516E-3</v>
       </c>
@@ -6360,7 +7430,7 @@
       <c r="Q56">
         <v>2.6</v>
       </c>
-      <c r="R56" s="17">
+      <c r="R56" s="16">
         <f t="shared" si="10"/>
         <v>41.602807999999641</v>
       </c>
@@ -6372,7 +7442,7 @@
       <c r="Q57">
         <v>2.7</v>
       </c>
-      <c r="R57" s="17">
+      <c r="R57" s="16">
         <f t="shared" si="10"/>
         <v>82.802438999999595</v>
       </c>
@@ -6384,7 +7454,7 @@
       <c r="Q58">
         <v>2.8</v>
       </c>
-      <c r="R58" s="17">
+      <c r="R58" s="16">
         <f t="shared" si="10"/>
         <v>123.20201599999973</v>
       </c>
@@ -6396,7 +7466,7 @@
       <c r="Q59">
         <v>2.9</v>
       </c>
-      <c r="R59" s="17">
+      <c r="R59" s="16">
         <f t="shared" si="10"/>
         <v>162.40153699999973</v>
       </c>
@@ -6408,7 +7478,7 @@
       <c r="Q60">
         <v>3</v>
       </c>
-      <c r="R60" s="17">
+      <c r="R60" s="16">
         <f t="shared" si="10"/>
         <v>200.00099999999975</v>
       </c>
@@ -6420,7 +7490,7 @@
       <c r="Q61">
         <v>3.1</v>
       </c>
-      <c r="R61" s="17">
+      <c r="R61" s="16">
         <f t="shared" si="10"/>
         <v>235.60040300000037</v>
       </c>
@@ -6432,7 +7502,7 @@
       <c r="Q62">
         <v>3.2</v>
       </c>
-      <c r="R62" s="17">
+      <c r="R62" s="16">
         <f t="shared" si="10"/>
         <v>268.79974399999992</v>
       </c>
@@ -6444,7 +7514,7 @@
       <c r="Q63">
         <v>3.3</v>
       </c>
-      <c r="R63" s="17">
+      <c r="R63" s="16">
         <f t="shared" si="10"/>
         <v>299.19902099999899</v>
       </c>
@@ -6456,7 +7526,7 @@
       <c r="Q64">
         <v>3.4</v>
       </c>
-      <c r="R64" s="17">
+      <c r="R64" s="16">
         <f t="shared" si="10"/>
         <v>326.3982319999991</v>
       </c>
@@ -6468,7 +7538,7 @@
       <c r="Q65">
         <v>3.5</v>
       </c>
-      <c r="R65" s="17">
+      <c r="R65" s="16">
         <f t="shared" si="10"/>
         <v>349.99737499999992</v>
       </c>
@@ -6480,7 +7550,7 @@
       <c r="Q66">
         <v>3.6</v>
       </c>
-      <c r="R66" s="17">
+      <c r="R66" s="16">
         <f t="shared" si="10"/>
         <v>369.59644799999933</v>
       </c>
@@ -6492,7 +7562,7 @@
       <c r="Q67">
         <v>3.7</v>
       </c>
-      <c r="R67" s="17">
+      <c r="R67" s="16">
         <f t="shared" si="10"/>
         <v>384.79544900000019</v>
       </c>
@@ -6504,7 +7574,7 @@
       <c r="Q68">
         <v>3.8</v>
       </c>
-      <c r="R68" s="17">
+      <c r="R68" s="16">
         <f t="shared" si="10"/>
         <v>395.19437600000037</v>
       </c>
@@ -6516,7 +7586,7 @@
       <c r="Q69">
         <v>3.9</v>
       </c>
-      <c r="R69" s="17">
+      <c r="R69" s="16">
         <f t="shared" si="10"/>
         <v>400.39322699999911</v>
       </c>
@@ -6528,7 +7598,7 @@
       <c r="Q70">
         <v>4</v>
       </c>
-      <c r="R70" s="17">
+      <c r="R70" s="16">
         <f t="shared" si="10"/>
         <v>399.99199999999973</v>
       </c>
@@ -6537,128 +7607,240 @@
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
       <c r="I71" s="2"/>
+      <c r="Q71">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="R71" s="16">
+        <f t="shared" ref="R71:R86" si="15" xml:space="preserve"> -66.667*POWER(Q71,3) + 500*POWER(Q71,2) - 833.33*Q71</f>
+        <v>393.59069300000056</v>
+      </c>
     </row>
     <row r="72" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
       <c r="I72" s="2"/>
+      <c r="Q72">
+        <v>4.2</v>
+      </c>
+      <c r="R72" s="16">
+        <f t="shared" si="15"/>
+        <v>380.78930399999945</v>
+      </c>
     </row>
     <row r="73" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="I73" s="2"/>
+      <c r="Q73">
+        <v>4.3</v>
+      </c>
+      <c r="R73" s="16">
+        <f t="shared" si="15"/>
+        <v>361.18783100000064</v>
+      </c>
     </row>
     <row r="74" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
       <c r="I74" s="2"/>
+      <c r="Q74">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="R74" s="16">
+        <f t="shared" si="15"/>
+        <v>334.38627199999928</v>
+      </c>
     </row>
     <row r="75" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
       <c r="I75" s="2"/>
+      <c r="Q75">
+        <v>4.5</v>
+      </c>
+      <c r="R75" s="16">
+        <f t="shared" si="15"/>
+        <v>299.9846249999996</v>
+      </c>
     </row>
     <row r="76" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="I76" s="2"/>
+      <c r="Q76">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="R76" s="16">
+        <f t="shared" si="15"/>
+        <v>257.58288800000037</v>
+      </c>
     </row>
     <row r="77" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
       <c r="I77" s="2"/>
+      <c r="Q77">
+        <v>4.7</v>
+      </c>
+      <c r="R77" s="16">
+        <f t="shared" si="15"/>
+        <v>206.78105899999946</v>
+      </c>
     </row>
     <row r="78" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="I78" s="2"/>
+      <c r="Q78">
+        <v>4.8</v>
+      </c>
+      <c r="R78" s="16">
+        <f t="shared" si="15"/>
+        <v>147.1791360000002</v>
+      </c>
     </row>
     <row r="79" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
       <c r="I79" s="2"/>
+      <c r="Q79">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="R79" s="16">
+        <f t="shared" si="15"/>
+        <v>78.377116999999544</v>
+      </c>
     </row>
     <row r="80" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="I80" s="2"/>
-    </row>
-    <row r="81" spans="5:9" x14ac:dyDescent="0.35">
+      <c r="Q80">
+        <v>5</v>
+      </c>
+      <c r="R80" s="16">
+        <f t="shared" si="15"/>
+        <v>-2.5000000000545697E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="I81" s="2"/>
-    </row>
-    <row r="82" spans="5:9" x14ac:dyDescent="0.35">
+      <c r="Q81">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="R81" s="16">
+        <f t="shared" si="15"/>
+        <v>-88.427217000000383</v>
+      </c>
+    </row>
+    <row r="82" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="I82" s="2"/>
-    </row>
-    <row r="83" spans="5:9" x14ac:dyDescent="0.35">
+      <c r="Q82">
+        <v>5.2</v>
+      </c>
+      <c r="R82" s="16">
+        <f t="shared" si="15"/>
+        <v>-187.22953600000073</v>
+      </c>
+    </row>
+    <row r="83" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
       <c r="I83" s="2"/>
-    </row>
-    <row r="84" spans="5:9" x14ac:dyDescent="0.35">
+      <c r="Q83">
+        <v>5.3</v>
+      </c>
+      <c r="R83" s="16">
+        <f t="shared" si="15"/>
+        <v>-296.8319590000001</v>
+      </c>
+    </row>
+    <row r="84" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="I84" s="2"/>
-    </row>
-    <row r="85" spans="5:9" x14ac:dyDescent="0.35">
+      <c r="Q84">
+        <v>5.4</v>
+      </c>
+      <c r="R84" s="16">
+        <f t="shared" si="15"/>
+        <v>-417.6344880000006</v>
+      </c>
+    </row>
+    <row r="85" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="I85" s="2"/>
-    </row>
-    <row r="86" spans="5:9" x14ac:dyDescent="0.35">
+      <c r="Q85">
+        <v>5.5</v>
+      </c>
+      <c r="R85" s="16">
+        <f t="shared" si="15"/>
+        <v>-550.03712500000074</v>
+      </c>
+    </row>
+    <row r="86" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
       <c r="I86" s="2"/>
-    </row>
-    <row r="87" spans="5:9" x14ac:dyDescent="0.35">
+      <c r="Q86">
+        <v>5.6</v>
+      </c>
+      <c r="R86" s="16">
+        <f t="shared" si="15"/>
+        <v>-694.43987199999992</v>
+      </c>
+    </row>
+    <row r="87" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
       <c r="I87" s="2"/>
     </row>
-    <row r="88" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="I88" s="2"/>
     </row>
-    <row r="89" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
       <c r="I89" s="2"/>
     </row>
-    <row r="90" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
       <c r="I90" s="2"/>
     </row>
-    <row r="91" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
       <c r="I91" s="2"/>
     </row>
-    <row r="92" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
       <c r="I92" s="2"/>
     </row>
-    <row r="93" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
       <c r="I93" s="2"/>
     </row>
-    <row r="94" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
       <c r="I94" s="2"/>
     </row>
-    <row r="95" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
       <c r="I95" s="2"/>
     </row>
-    <row r="96" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
       <c r="I96" s="2"/>
@@ -7913,4 +9095,157 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>500</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <f>A1/60</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1.5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <f>A7/A5/A3</f>
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <f>400/1</f>
+        <v>400</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <f>A2*A3*A5</f>
+        <v>5000</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <f>1800*2</f>
+        <v>3600</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <f>A2*A7</f>
+        <v>30000.000000000004</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <f>A3/A7</f>
+        <v>4.1666666666666669E-4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="18">
+        <f>A14/A5</f>
+        <v>0.05</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <f>A15/A11</f>
+        <v>120</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <f>1366/100000</f>
+        <v>1.366E-2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <f>A2*A18</f>
+        <v>0.11383333333333334</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <f>A19*A7</f>
+        <v>409.8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <f>A20*A11</f>
+        <v>0.17075000000000001</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>